<commit_message>
Project Updated at: 2024-07-04 21-53-04
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5787539" uniqueCount="12098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5795004" uniqueCount="12099">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41031,6 +41031,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId3959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatura</t>
   </si>
 </sst>
 </file>
@@ -58410,16 +58413,16 @@
         <v>45</v>
       </c>
       <c r="F595" t="s">
-        <v>12095</v>
+        <v>12098</v>
       </c>
       <c r="G595" t="s">
-        <v>11458</v>
+        <v>12098</v>
       </c>
       <c r="H595" t="s">
-        <v>11458</v>
+        <v>12098</v>
       </c>
       <c r="I595" t="s">
-        <v>11458</v>
+        <v>12098</v>
       </c>
     </row>
     <row r="596">
@@ -58439,13 +58442,13 @@
         <v>11534</v>
       </c>
       <c r="G596" t="s">
-        <v>11461</v>
+        <v>11534</v>
       </c>
       <c r="H596" t="s">
-        <v>11461</v>
+        <v>11534</v>
       </c>
       <c r="I596" t="s">
-        <v>11461</v>
+        <v>11534</v>
       </c>
     </row>
     <row r="597">
@@ -58491,13 +58494,13 @@
         <v>11537</v>
       </c>
       <c r="G598" t="s">
-        <v>11463</v>
+        <v>11537</v>
       </c>
       <c r="H598" t="s">
-        <v>11463</v>
+        <v>11537</v>
       </c>
       <c r="I598" t="s">
-        <v>11463</v>
+        <v>11537</v>
       </c>
     </row>
     <row r="599">
@@ -58621,13 +58624,13 @@
         <v>11930</v>
       </c>
       <c r="G603" t="s">
-        <v>47</v>
+        <v>11930</v>
       </c>
       <c r="H603" t="s">
-        <v>47</v>
+        <v>11930</v>
       </c>
       <c r="I603" t="s">
-        <v>47</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="604">

</xml_diff>

<commit_message>
Project Updated at: 2024-07-11 22-31-05
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5795004" uniqueCount="12099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5935062" uniqueCount="12205">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41034,6 +41034,369 @@
   </si>
   <si>
     <t xml:space="preserve">Temperatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGIENIZAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserir Senha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIR PORTA
+PARA COMEÇAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO PROCESSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA SAIR
+DO DEGELO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESEJA CANCELAR
+A HIGIENIZAÇÃO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-9999.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9999.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-999.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999.9</t>
   </si>
 </sst>
 </file>
@@ -58841,58 +59204,1358 @@
         <v>11550</v>
       </c>
     </row>
-    <row r="612"/>
-    <row r="613"/>
-    <row r="614"/>
-    <row r="615"/>
-    <row r="616"/>
-    <row r="617"/>
-    <row r="618"/>
-    <row r="619"/>
-    <row r="620"/>
-    <row r="621"/>
-    <row r="622"/>
-    <row r="623"/>
-    <row r="624"/>
-    <row r="625"/>
-    <row r="626"/>
-    <row r="627"/>
-    <row r="628"/>
-    <row r="629"/>
-    <row r="630"/>
-    <row r="631"/>
-    <row r="632"/>
-    <row r="633"/>
-    <row r="634"/>
-    <row r="635"/>
-    <row r="636"/>
-    <row r="637"/>
-    <row r="638"/>
-    <row r="639"/>
-    <row r="640"/>
-    <row r="641"/>
-    <row r="642"/>
-    <row r="643"/>
-    <row r="644"/>
-    <row r="645"/>
-    <row r="646"/>
-    <row r="647"/>
-    <row r="648"/>
-    <row r="649"/>
-    <row r="650"/>
-    <row r="651"/>
-    <row r="652"/>
-    <row r="653"/>
-    <row r="654"/>
-    <row r="655"/>
-    <row r="656"/>
-    <row r="657"/>
-    <row r="658"/>
-    <row r="659"/>
-    <row r="660"/>
-    <row r="661"/>
-    <row r="662"/>
-    <row r="663"/>
+    <row r="612">
+      <c r="B612" t="s">
+        <v>12099</v>
+      </c>
+      <c r="C612" t="s">
+        <v>77</v>
+      </c>
+      <c r="D612" t="s">
+        <v>44</v>
+      </c>
+      <c r="E612" t="s">
+        <v>45</v>
+      </c>
+      <c r="F612" t="s">
+        <v>12100</v>
+      </c>
+      <c r="G612" t="s">
+        <v>12100</v>
+      </c>
+      <c r="H612" t="s">
+        <v>12100</v>
+      </c>
+      <c r="I612" t="s">
+        <v>12100</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="B613" t="s">
+        <v>12101</v>
+      </c>
+      <c r="C613" t="s">
+        <v>40</v>
+      </c>
+      <c r="D613" t="s">
+        <v>49</v>
+      </c>
+      <c r="E613" t="s">
+        <v>45</v>
+      </c>
+      <c r="F613" t="s">
+        <v>12102</v>
+      </c>
+      <c r="G613" t="s">
+        <v>12102</v>
+      </c>
+      <c r="H613" t="s">
+        <v>12102</v>
+      </c>
+      <c r="I613" t="s">
+        <v>12102</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="B614" t="s">
+        <v>12104</v>
+      </c>
+      <c r="C614" t="s">
+        <v>78</v>
+      </c>
+      <c r="D614" t="s">
+        <v>44</v>
+      </c>
+      <c r="E614" t="s">
+        <v>45</v>
+      </c>
+      <c r="F614" t="s">
+        <v>1574</v>
+      </c>
+      <c r="G614" t="s">
+        <v>1574</v>
+      </c>
+      <c r="H614" t="s">
+        <v>1574</v>
+      </c>
+      <c r="I614" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="B615" t="s">
+        <v>12105</v>
+      </c>
+      <c r="C615" t="s">
+        <v>77</v>
+      </c>
+      <c r="D615" t="s">
+        <v>44</v>
+      </c>
+      <c r="E615" t="s">
+        <v>45</v>
+      </c>
+      <c r="F615" t="s">
+        <v>11458</v>
+      </c>
+      <c r="G615" t="s">
+        <v>11458</v>
+      </c>
+      <c r="H615" t="s">
+        <v>11458</v>
+      </c>
+      <c r="I615" t="s">
+        <v>11458</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="B616" t="s">
+        <v>12106</v>
+      </c>
+      <c r="C616" t="s">
+        <v>101</v>
+      </c>
+      <c r="D616" t="s">
+        <v>44</v>
+      </c>
+      <c r="E616" t="s">
+        <v>45</v>
+      </c>
+      <c r="F616" t="s">
+        <v>11462</v>
+      </c>
+      <c r="G616" t="s">
+        <v>11462</v>
+      </c>
+      <c r="H616" t="s">
+        <v>11462</v>
+      </c>
+      <c r="I616" t="s">
+        <v>11462</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="B617" t="s">
+        <v>12107</v>
+      </c>
+      <c r="C617" t="s">
+        <v>77</v>
+      </c>
+      <c r="D617" t="s">
+        <v>49</v>
+      </c>
+      <c r="E617" t="s">
+        <v>45</v>
+      </c>
+      <c r="F617" t="s">
+        <v>50</v>
+      </c>
+      <c r="G617" t="s">
+        <v>50</v>
+      </c>
+      <c r="H617" t="s">
+        <v>50</v>
+      </c>
+      <c r="I617" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="B618" t="s">
+        <v>12108</v>
+      </c>
+      <c r="C618" t="s">
+        <v>77</v>
+      </c>
+      <c r="D618" t="s">
+        <v>44</v>
+      </c>
+      <c r="E618" t="s">
+        <v>45</v>
+      </c>
+      <c r="F618" t="s">
+        <v>11512</v>
+      </c>
+      <c r="G618" t="s">
+        <v>11512</v>
+      </c>
+      <c r="H618" t="s">
+        <v>11512</v>
+      </c>
+      <c r="I618" t="s">
+        <v>11512</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="B619" t="s">
+        <v>12109</v>
+      </c>
+      <c r="C619" t="s">
+        <v>11926</v>
+      </c>
+      <c r="D619" t="s">
+        <v>44</v>
+      </c>
+      <c r="E619" t="s">
+        <v>45</v>
+      </c>
+      <c r="F619" t="s">
+        <v>11930</v>
+      </c>
+      <c r="G619" t="s">
+        <v>47</v>
+      </c>
+      <c r="H619" t="s">
+        <v>47</v>
+      </c>
+      <c r="I619" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="B620" t="s">
+        <v>12110</v>
+      </c>
+      <c r="C620" t="s">
+        <v>101</v>
+      </c>
+      <c r="D620" t="s">
+        <v>49</v>
+      </c>
+      <c r="E620" t="s">
+        <v>45</v>
+      </c>
+      <c r="F620" t="s">
+        <v>50</v>
+      </c>
+      <c r="G620" t="s">
+        <v>50</v>
+      </c>
+      <c r="H620" t="s">
+        <v>50</v>
+      </c>
+      <c r="I620" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="B621" t="s">
+        <v>12111</v>
+      </c>
+      <c r="C621" t="s">
+        <v>101</v>
+      </c>
+      <c r="D621" t="s">
+        <v>44</v>
+      </c>
+      <c r="E621" t="s">
+        <v>45</v>
+      </c>
+      <c r="F621" t="s">
+        <v>11510</v>
+      </c>
+      <c r="G621" t="s">
+        <v>11510</v>
+      </c>
+      <c r="H621" t="s">
+        <v>11510</v>
+      </c>
+      <c r="I621" t="s">
+        <v>11510</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="B622" t="s">
+        <v>12114</v>
+      </c>
+      <c r="C622" t="s">
+        <v>77</v>
+      </c>
+      <c r="D622" t="s">
+        <v>49</v>
+      </c>
+      <c r="E622" t="s">
+        <v>45</v>
+      </c>
+      <c r="F622" t="s">
+        <v>2570</v>
+      </c>
+      <c r="G622" t="s">
+        <v>2570</v>
+      </c>
+      <c r="H622" t="s">
+        <v>2570</v>
+      </c>
+      <c r="I622" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="B623" t="s">
+        <v>12115</v>
+      </c>
+      <c r="C623" t="s">
+        <v>77</v>
+      </c>
+      <c r="D623" t="s">
+        <v>49</v>
+      </c>
+      <c r="E623" t="s">
+        <v>45</v>
+      </c>
+      <c r="F623" t="s">
+        <v>2574</v>
+      </c>
+      <c r="G623" t="s">
+        <v>2574</v>
+      </c>
+      <c r="H623" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I623" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="B624" t="s">
+        <v>12116</v>
+      </c>
+      <c r="C624" t="s">
+        <v>77</v>
+      </c>
+      <c r="D624" t="s">
+        <v>49</v>
+      </c>
+      <c r="E624" t="s">
+        <v>45</v>
+      </c>
+      <c r="F624" t="s">
+        <v>12117</v>
+      </c>
+      <c r="G624" t="s">
+        <v>12117</v>
+      </c>
+      <c r="H624" t="s">
+        <v>12117</v>
+      </c>
+      <c r="I624" t="s">
+        <v>12117</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="B625" t="s">
+        <v>12120</v>
+      </c>
+      <c r="C625" t="s">
+        <v>77</v>
+      </c>
+      <c r="D625" t="s">
+        <v>49</v>
+      </c>
+      <c r="E625" t="s">
+        <v>45</v>
+      </c>
+      <c r="F625" t="s">
+        <v>2574</v>
+      </c>
+      <c r="G625" t="s">
+        <v>2574</v>
+      </c>
+      <c r="H625" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I625" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="B626" t="s">
+        <v>12121</v>
+      </c>
+      <c r="C626" t="s">
+        <v>77</v>
+      </c>
+      <c r="D626" t="s">
+        <v>49</v>
+      </c>
+      <c r="E626" t="s">
+        <v>45</v>
+      </c>
+      <c r="F626" t="s">
+        <v>2570</v>
+      </c>
+      <c r="G626" t="s">
+        <v>2570</v>
+      </c>
+      <c r="H626" t="s">
+        <v>2570</v>
+      </c>
+      <c r="I626" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="B627" t="s">
+        <v>12122</v>
+      </c>
+      <c r="C627" t="s">
+        <v>77</v>
+      </c>
+      <c r="D627" t="s">
+        <v>49</v>
+      </c>
+      <c r="E627" t="s">
+        <v>45</v>
+      </c>
+      <c r="F627" t="s">
+        <v>12123</v>
+      </c>
+      <c r="G627" t="s">
+        <v>12123</v>
+      </c>
+      <c r="H627" t="s">
+        <v>12123</v>
+      </c>
+      <c r="I627" t="s">
+        <v>12123</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="B628" t="s">
+        <v>12124</v>
+      </c>
+      <c r="C628" t="s">
+        <v>78</v>
+      </c>
+      <c r="D628" t="s">
+        <v>49</v>
+      </c>
+      <c r="E628" t="s">
+        <v>45</v>
+      </c>
+      <c r="F628" t="s">
+        <v>2450</v>
+      </c>
+      <c r="G628" t="s">
+        <v>2450</v>
+      </c>
+      <c r="H628" t="s">
+        <v>2450</v>
+      </c>
+      <c r="I628" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="B629" t="s">
+        <v>12125</v>
+      </c>
+      <c r="C629" t="s">
+        <v>78</v>
+      </c>
+      <c r="D629" t="s">
+        <v>49</v>
+      </c>
+      <c r="E629" t="s">
+        <v>45</v>
+      </c>
+      <c r="F629" t="s">
+        <v>12126</v>
+      </c>
+      <c r="G629" t="s">
+        <v>12126</v>
+      </c>
+      <c r="H629" t="s">
+        <v>12126</v>
+      </c>
+      <c r="I629" t="s">
+        <v>12126</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="B630" t="s">
+        <v>12127</v>
+      </c>
+      <c r="C630" t="s">
+        <v>77</v>
+      </c>
+      <c r="D630" t="s">
+        <v>49</v>
+      </c>
+      <c r="E630" t="s">
+        <v>45</v>
+      </c>
+      <c r="F630" t="s">
+        <v>12128</v>
+      </c>
+      <c r="G630" t="s">
+        <v>12128</v>
+      </c>
+      <c r="H630" t="s">
+        <v>12128</v>
+      </c>
+      <c r="I630" t="s">
+        <v>12128</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="B631" t="s">
+        <v>12129</v>
+      </c>
+      <c r="C631" t="s">
+        <v>78</v>
+      </c>
+      <c r="D631" t="s">
+        <v>49</v>
+      </c>
+      <c r="E631" t="s">
+        <v>45</v>
+      </c>
+      <c r="F631" t="s">
+        <v>50</v>
+      </c>
+      <c r="G631" t="s">
+        <v>50</v>
+      </c>
+      <c r="H631" t="s">
+        <v>50</v>
+      </c>
+      <c r="I631" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="B632" t="s">
+        <v>12130</v>
+      </c>
+      <c r="C632" t="s">
+        <v>78</v>
+      </c>
+      <c r="D632" t="s">
+        <v>44</v>
+      </c>
+      <c r="E632" t="s">
+        <v>45</v>
+      </c>
+      <c r="F632" t="s">
+        <v>12131</v>
+      </c>
+      <c r="G632" t="s">
+        <v>12131</v>
+      </c>
+      <c r="H632" t="s">
+        <v>12131</v>
+      </c>
+      <c r="I632" t="s">
+        <v>12131</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="B633" t="s">
+        <v>12132</v>
+      </c>
+      <c r="C633" t="s">
+        <v>77</v>
+      </c>
+      <c r="D633" t="s">
+        <v>49</v>
+      </c>
+      <c r="E633" t="s">
+        <v>45</v>
+      </c>
+      <c r="F633" t="s">
+        <v>2574</v>
+      </c>
+      <c r="G633" t="s">
+        <v>2574</v>
+      </c>
+      <c r="H633" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I633" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="B634" t="s">
+        <v>12133</v>
+      </c>
+      <c r="C634" t="s">
+        <v>77</v>
+      </c>
+      <c r="D634" t="s">
+        <v>49</v>
+      </c>
+      <c r="E634" t="s">
+        <v>45</v>
+      </c>
+      <c r="F634" t="s">
+        <v>2570</v>
+      </c>
+      <c r="G634" t="s">
+        <v>2570</v>
+      </c>
+      <c r="H634" t="s">
+        <v>2570</v>
+      </c>
+      <c r="I634" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="B635" t="s">
+        <v>12134</v>
+      </c>
+      <c r="C635" t="s">
+        <v>77</v>
+      </c>
+      <c r="D635" t="s">
+        <v>49</v>
+      </c>
+      <c r="E635" t="s">
+        <v>45</v>
+      </c>
+      <c r="F635" t="s">
+        <v>12135</v>
+      </c>
+      <c r="G635" t="s">
+        <v>12135</v>
+      </c>
+      <c r="H635" t="s">
+        <v>12135</v>
+      </c>
+      <c r="I635" t="s">
+        <v>12135</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="B636" t="s">
+        <v>12148</v>
+      </c>
+      <c r="C636" t="s">
+        <v>77</v>
+      </c>
+      <c r="D636" t="s">
+        <v>49</v>
+      </c>
+      <c r="E636" t="s">
+        <v>45</v>
+      </c>
+      <c r="F636" t="s">
+        <v>50</v>
+      </c>
+      <c r="G636" t="s">
+        <v>50</v>
+      </c>
+      <c r="H636" t="s">
+        <v>50</v>
+      </c>
+      <c r="I636" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="B637" t="s">
+        <v>12149</v>
+      </c>
+      <c r="C637" t="s">
+        <v>77</v>
+      </c>
+      <c r="D637" t="s">
+        <v>44</v>
+      </c>
+      <c r="E637" t="s">
+        <v>45</v>
+      </c>
+      <c r="F637" t="s">
+        <v>11550</v>
+      </c>
+      <c r="G637" t="s">
+        <v>11550</v>
+      </c>
+      <c r="H637" t="s">
+        <v>11550</v>
+      </c>
+      <c r="I637" t="s">
+        <v>11550</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="B638" t="s">
+        <v>12150</v>
+      </c>
+      <c r="C638" t="s">
+        <v>78</v>
+      </c>
+      <c r="D638" t="s">
+        <v>44</v>
+      </c>
+      <c r="E638" t="s">
+        <v>45</v>
+      </c>
+      <c r="F638" t="s">
+        <v>12048</v>
+      </c>
+      <c r="G638" t="s">
+        <v>12048</v>
+      </c>
+      <c r="H638" t="s">
+        <v>12048</v>
+      </c>
+      <c r="I638" t="s">
+        <v>12048</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="B639" t="s">
+        <v>12151</v>
+      </c>
+      <c r="C639" t="s">
+        <v>78</v>
+      </c>
+      <c r="D639" t="s">
+        <v>44</v>
+      </c>
+      <c r="E639" t="s">
+        <v>45</v>
+      </c>
+      <c r="F639" t="s">
+        <v>12152</v>
+      </c>
+      <c r="G639" t="s">
+        <v>12152</v>
+      </c>
+      <c r="H639" t="s">
+        <v>12152</v>
+      </c>
+      <c r="I639" t="s">
+        <v>12152</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="B640" t="s">
+        <v>12153</v>
+      </c>
+      <c r="C640" t="s">
+        <v>78</v>
+      </c>
+      <c r="D640" t="s">
+        <v>49</v>
+      </c>
+      <c r="E640" t="s">
+        <v>45</v>
+      </c>
+      <c r="F640" t="s">
+        <v>50</v>
+      </c>
+      <c r="G640" t="s">
+        <v>50</v>
+      </c>
+      <c r="H640" t="s">
+        <v>50</v>
+      </c>
+      <c r="I640" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="B641" t="s">
+        <v>12154</v>
+      </c>
+      <c r="C641" t="s">
+        <v>78</v>
+      </c>
+      <c r="D641" t="s">
+        <v>44</v>
+      </c>
+      <c r="E641" t="s">
+        <v>45</v>
+      </c>
+      <c r="F641" t="s">
+        <v>11780</v>
+      </c>
+      <c r="G641" t="s">
+        <v>11780</v>
+      </c>
+      <c r="H641" t="s">
+        <v>11780</v>
+      </c>
+      <c r="I641" t="s">
+        <v>11780</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="B642" t="s">
+        <v>12179</v>
+      </c>
+      <c r="C642" t="s">
+        <v>77</v>
+      </c>
+      <c r="D642" t="s">
+        <v>49</v>
+      </c>
+      <c r="E642" t="s">
+        <v>45</v>
+      </c>
+      <c r="F642" t="s">
+        <v>50</v>
+      </c>
+      <c r="G642" t="s">
+        <v>50</v>
+      </c>
+      <c r="H642" t="s">
+        <v>50</v>
+      </c>
+      <c r="I642" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="B643" t="s">
+        <v>12180</v>
+      </c>
+      <c r="C643" t="s">
+        <v>77</v>
+      </c>
+      <c r="D643" t="s">
+        <v>44</v>
+      </c>
+      <c r="E643" t="s">
+        <v>45</v>
+      </c>
+      <c r="F643" t="s">
+        <v>52</v>
+      </c>
+      <c r="G643" t="s">
+        <v>284</v>
+      </c>
+      <c r="H643" t="s">
+        <v>284</v>
+      </c>
+      <c r="I643" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="B644" t="s">
+        <v>12181</v>
+      </c>
+      <c r="C644" t="s">
+        <v>38</v>
+      </c>
+      <c r="D644" t="s">
+        <v>49</v>
+      </c>
+      <c r="E644" t="s">
+        <v>45</v>
+      </c>
+      <c r="F644" t="s">
+        <v>390</v>
+      </c>
+      <c r="G644" t="s">
+        <v>390</v>
+      </c>
+      <c r="H644" t="s">
+        <v>390</v>
+      </c>
+      <c r="I644" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="B645" t="s">
+        <v>12182</v>
+      </c>
+      <c r="C645" t="s">
+        <v>38</v>
+      </c>
+      <c r="D645" t="s">
+        <v>49</v>
+      </c>
+      <c r="E645" t="s">
+        <v>45</v>
+      </c>
+      <c r="F645" t="s">
+        <v>319</v>
+      </c>
+      <c r="G645" t="s">
+        <v>319</v>
+      </c>
+      <c r="H645" t="s">
+        <v>319</v>
+      </c>
+      <c r="I645" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="B646" t="s">
+        <v>12183</v>
+      </c>
+      <c r="C646" t="s">
+        <v>38</v>
+      </c>
+      <c r="D646" t="s">
+        <v>49</v>
+      </c>
+      <c r="E646" t="s">
+        <v>45</v>
+      </c>
+      <c r="F646" t="s">
+        <v>504</v>
+      </c>
+      <c r="G646" t="s">
+        <v>504</v>
+      </c>
+      <c r="H646" t="s">
+        <v>504</v>
+      </c>
+      <c r="I646" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="B647" t="s">
+        <v>12184</v>
+      </c>
+      <c r="C647" t="s">
+        <v>38</v>
+      </c>
+      <c r="D647" t="s">
+        <v>49</v>
+      </c>
+      <c r="E647" t="s">
+        <v>45</v>
+      </c>
+      <c r="F647" t="s">
+        <v>506</v>
+      </c>
+      <c r="G647" t="s">
+        <v>506</v>
+      </c>
+      <c r="H647" t="s">
+        <v>506</v>
+      </c>
+      <c r="I647" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="B648" t="s">
+        <v>12185</v>
+      </c>
+      <c r="C648" t="s">
+        <v>38</v>
+      </c>
+      <c r="D648" t="s">
+        <v>49</v>
+      </c>
+      <c r="E648" t="s">
+        <v>45</v>
+      </c>
+      <c r="F648" t="s">
+        <v>508</v>
+      </c>
+      <c r="G648" t="s">
+        <v>508</v>
+      </c>
+      <c r="H648" t="s">
+        <v>508</v>
+      </c>
+      <c r="I648" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="B649" t="s">
+        <v>12186</v>
+      </c>
+      <c r="C649" t="s">
+        <v>38</v>
+      </c>
+      <c r="D649" t="s">
+        <v>49</v>
+      </c>
+      <c r="E649" t="s">
+        <v>45</v>
+      </c>
+      <c r="F649" t="s">
+        <v>510</v>
+      </c>
+      <c r="G649" t="s">
+        <v>510</v>
+      </c>
+      <c r="H649" t="s">
+        <v>510</v>
+      </c>
+      <c r="I649" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="B650" t="s">
+        <v>12187</v>
+      </c>
+      <c r="C650" t="s">
+        <v>38</v>
+      </c>
+      <c r="D650" t="s">
+        <v>49</v>
+      </c>
+      <c r="E650" t="s">
+        <v>45</v>
+      </c>
+      <c r="F650" t="s">
+        <v>512</v>
+      </c>
+      <c r="G650" t="s">
+        <v>512</v>
+      </c>
+      <c r="H650" t="s">
+        <v>512</v>
+      </c>
+      <c r="I650" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="B651" t="s">
+        <v>12188</v>
+      </c>
+      <c r="C651" t="s">
+        <v>38</v>
+      </c>
+      <c r="D651" t="s">
+        <v>49</v>
+      </c>
+      <c r="E651" t="s">
+        <v>45</v>
+      </c>
+      <c r="F651" t="s">
+        <v>514</v>
+      </c>
+      <c r="G651" t="s">
+        <v>514</v>
+      </c>
+      <c r="H651" t="s">
+        <v>514</v>
+      </c>
+      <c r="I651" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="B652" t="s">
+        <v>12189</v>
+      </c>
+      <c r="C652" t="s">
+        <v>38</v>
+      </c>
+      <c r="D652" t="s">
+        <v>49</v>
+      </c>
+      <c r="E652" t="s">
+        <v>45</v>
+      </c>
+      <c r="F652" t="s">
+        <v>516</v>
+      </c>
+      <c r="G652" t="s">
+        <v>516</v>
+      </c>
+      <c r="H652" t="s">
+        <v>516</v>
+      </c>
+      <c r="I652" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="B653" t="s">
+        <v>12190</v>
+      </c>
+      <c r="C653" t="s">
+        <v>38</v>
+      </c>
+      <c r="D653" t="s">
+        <v>49</v>
+      </c>
+      <c r="E653" t="s">
+        <v>45</v>
+      </c>
+      <c r="F653" t="s">
+        <v>522</v>
+      </c>
+      <c r="G653" t="s">
+        <v>522</v>
+      </c>
+      <c r="H653" t="s">
+        <v>522</v>
+      </c>
+      <c r="I653" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="B654" t="s">
+        <v>12191</v>
+      </c>
+      <c r="C654" t="s">
+        <v>38</v>
+      </c>
+      <c r="D654" t="s">
+        <v>49</v>
+      </c>
+      <c r="E654" t="s">
+        <v>45</v>
+      </c>
+      <c r="F654" t="s">
+        <v>1278</v>
+      </c>
+      <c r="G654" t="s">
+        <v>1278</v>
+      </c>
+      <c r="H654" t="s">
+        <v>1278</v>
+      </c>
+      <c r="I654" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="B655" t="s">
+        <v>12192</v>
+      </c>
+      <c r="C655" t="s">
+        <v>38</v>
+      </c>
+      <c r="D655" t="s">
+        <v>49</v>
+      </c>
+      <c r="E655" t="s">
+        <v>45</v>
+      </c>
+      <c r="F655" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G655" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H655" t="s">
+        <v>1279</v>
+      </c>
+      <c r="I655" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="B656" t="s">
+        <v>12193</v>
+      </c>
+      <c r="C656" t="s">
+        <v>38</v>
+      </c>
+      <c r="D656" t="s">
+        <v>49</v>
+      </c>
+      <c r="E656" t="s">
+        <v>45</v>
+      </c>
+      <c r="F656" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G656" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H656" t="s">
+        <v>1280</v>
+      </c>
+      <c r="I656" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="B657" t="s">
+        <v>12194</v>
+      </c>
+      <c r="C657" t="s">
+        <v>38</v>
+      </c>
+      <c r="D657" t="s">
+        <v>49</v>
+      </c>
+      <c r="E657" t="s">
+        <v>45</v>
+      </c>
+      <c r="F657" t="s">
+        <v>1281</v>
+      </c>
+      <c r="G657" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H657" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I657" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="B658" t="s">
+        <v>12195</v>
+      </c>
+      <c r="C658" t="s">
+        <v>101</v>
+      </c>
+      <c r="D658" t="s">
+        <v>49</v>
+      </c>
+      <c r="E658" t="s">
+        <v>45</v>
+      </c>
+      <c r="F658" t="s">
+        <v>313</v>
+      </c>
+      <c r="G658" t="s">
+        <v>313</v>
+      </c>
+      <c r="H658" t="s">
+        <v>313</v>
+      </c>
+      <c r="I658" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="B659" t="s">
+        <v>12196</v>
+      </c>
+      <c r="C659" t="s">
+        <v>101</v>
+      </c>
+      <c r="D659" t="s">
+        <v>49</v>
+      </c>
+      <c r="E659" t="s">
+        <v>45</v>
+      </c>
+      <c r="F659" t="s">
+        <v>1631</v>
+      </c>
+      <c r="G659" t="s">
+        <v>1631</v>
+      </c>
+      <c r="H659" t="s">
+        <v>1631</v>
+      </c>
+      <c r="I659" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="B660" t="s">
+        <v>12197</v>
+      </c>
+      <c r="C660" t="s">
+        <v>38</v>
+      </c>
+      <c r="D660" t="s">
+        <v>49</v>
+      </c>
+      <c r="E660" t="s">
+        <v>45</v>
+      </c>
+      <c r="F660" t="s">
+        <v>50</v>
+      </c>
+      <c r="G660" t="s">
+        <v>50</v>
+      </c>
+      <c r="H660" t="s">
+        <v>50</v>
+      </c>
+      <c r="I660" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="B661" t="s">
+        <v>12198</v>
+      </c>
+      <c r="C661" t="s">
+        <v>38</v>
+      </c>
+      <c r="D661" t="s">
+        <v>44</v>
+      </c>
+      <c r="E661" t="s">
+        <v>45</v>
+      </c>
+      <c r="F661" t="s">
+        <v>12203</v>
+      </c>
+      <c r="G661" t="s">
+        <v>52</v>
+      </c>
+      <c r="H661" t="s">
+        <v>52</v>
+      </c>
+      <c r="I661" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="B662" t="s">
+        <v>12199</v>
+      </c>
+      <c r="C662" t="s">
+        <v>38</v>
+      </c>
+      <c r="D662" t="s">
+        <v>49</v>
+      </c>
+      <c r="E662" t="s">
+        <v>45</v>
+      </c>
+      <c r="F662" t="s">
+        <v>50</v>
+      </c>
+      <c r="G662" t="s">
+        <v>50</v>
+      </c>
+      <c r="H662" t="s">
+        <v>50</v>
+      </c>
+      <c r="I662" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="B663" t="s">
+        <v>12200</v>
+      </c>
+      <c r="C663" t="s">
+        <v>38</v>
+      </c>
+      <c r="D663" t="s">
+        <v>44</v>
+      </c>
+      <c r="E663" t="s">
+        <v>45</v>
+      </c>
+      <c r="F663" t="s">
+        <v>12204</v>
+      </c>
+      <c r="G663" t="s">
+        <v>52</v>
+      </c>
+      <c r="H663" t="s">
+        <v>52</v>
+      </c>
+      <c r="I663" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="664"/>
     <row r="665"/>
     <row r="666"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-07-15 21-35-54
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5935062" uniqueCount="12205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5951240" uniqueCount="12207">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41397,6 +41397,12 @@
   </si>
   <si>
     <t xml:space="preserve">999.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desabilitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">888.88</t>
   </si>
 </sst>
 </file>
@@ -52900,7 +52906,7 @@
         <v>45</v>
       </c>
       <c r="F369" t="s">
-        <v>11508</v>
+        <v>12206</v>
       </c>
       <c r="G369" t="s">
         <v>11508</v>
@@ -53498,7 +53504,7 @@
         <v>45</v>
       </c>
       <c r="F392" t="s">
-        <v>11660</v>
+        <v>12205</v>
       </c>
       <c r="G392" t="s">
         <v>11660</v>

</xml_diff>

<commit_message>
Project Updated at: 2024-07-17 21-53-59
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5951240" uniqueCount="12207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5975279" uniqueCount="12209">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41403,6 +41403,12 @@
   </si>
   <si>
     <t xml:space="preserve">888.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edição de Receita &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4018</t>
   </si>
 </sst>
 </file>
@@ -57924,16 +57930,16 @@
         <v>45</v>
       </c>
       <c r="F562" t="s">
-        <v>12033</v>
+        <v>12207</v>
       </c>
       <c r="G562" t="s">
-        <v>12033</v>
+        <v>12207</v>
       </c>
       <c r="H562" t="s">
-        <v>12033</v>
+        <v>12207</v>
       </c>
       <c r="I562" t="s">
-        <v>12033</v>
+        <v>12207</v>
       </c>
     </row>
     <row r="563">
@@ -59992,576 +59998,51 @@
     </row>
     <row r="642">
       <c r="B642" t="s">
-        <v>12179</v>
+        <v>12208</v>
       </c>
       <c r="C642" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="D642" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E642" t="s">
         <v>45</v>
       </c>
       <c r="F642" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G642" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H642" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I642" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="643">
-      <c r="B643" t="s">
-        <v>12180</v>
-      </c>
-      <c r="C643" t="s">
-        <v>77</v>
-      </c>
-      <c r="D643" t="s">
-        <v>44</v>
-      </c>
-      <c r="E643" t="s">
-        <v>45</v>
-      </c>
-      <c r="F643" t="s">
-        <v>52</v>
-      </c>
-      <c r="G643" t="s">
         <v>284</v>
       </c>
-      <c r="H643" t="s">
-        <v>284</v>
-      </c>
-      <c r="I643" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="644">
-      <c r="B644" t="s">
-        <v>12181</v>
-      </c>
-      <c r="C644" t="s">
-        <v>38</v>
-      </c>
-      <c r="D644" t="s">
-        <v>49</v>
-      </c>
-      <c r="E644" t="s">
-        <v>45</v>
-      </c>
-      <c r="F644" t="s">
-        <v>390</v>
-      </c>
-      <c r="G644" t="s">
-        <v>390</v>
-      </c>
-      <c r="H644" t="s">
-        <v>390</v>
-      </c>
-      <c r="I644" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="645">
-      <c r="B645" t="s">
-        <v>12182</v>
-      </c>
-      <c r="C645" t="s">
-        <v>38</v>
-      </c>
-      <c r="D645" t="s">
-        <v>49</v>
-      </c>
-      <c r="E645" t="s">
-        <v>45</v>
-      </c>
-      <c r="F645" t="s">
-        <v>319</v>
-      </c>
-      <c r="G645" t="s">
-        <v>319</v>
-      </c>
-      <c r="H645" t="s">
-        <v>319</v>
-      </c>
-      <c r="I645" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="646">
-      <c r="B646" t="s">
-        <v>12183</v>
-      </c>
-      <c r="C646" t="s">
-        <v>38</v>
-      </c>
-      <c r="D646" t="s">
-        <v>49</v>
-      </c>
-      <c r="E646" t="s">
-        <v>45</v>
-      </c>
-      <c r="F646" t="s">
-        <v>504</v>
-      </c>
-      <c r="G646" t="s">
-        <v>504</v>
-      </c>
-      <c r="H646" t="s">
-        <v>504</v>
-      </c>
-      <c r="I646" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="647">
-      <c r="B647" t="s">
-        <v>12184</v>
-      </c>
-      <c r="C647" t="s">
-        <v>38</v>
-      </c>
-      <c r="D647" t="s">
-        <v>49</v>
-      </c>
-      <c r="E647" t="s">
-        <v>45</v>
-      </c>
-      <c r="F647" t="s">
-        <v>506</v>
-      </c>
-      <c r="G647" t="s">
-        <v>506</v>
-      </c>
-      <c r="H647" t="s">
-        <v>506</v>
-      </c>
-      <c r="I647" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="648">
-      <c r="B648" t="s">
-        <v>12185</v>
-      </c>
-      <c r="C648" t="s">
-        <v>38</v>
-      </c>
-      <c r="D648" t="s">
-        <v>49</v>
-      </c>
-      <c r="E648" t="s">
-        <v>45</v>
-      </c>
-      <c r="F648" t="s">
-        <v>508</v>
-      </c>
-      <c r="G648" t="s">
-        <v>508</v>
-      </c>
-      <c r="H648" t="s">
-        <v>508</v>
-      </c>
-      <c r="I648" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="649">
-      <c r="B649" t="s">
-        <v>12186</v>
-      </c>
-      <c r="C649" t="s">
-        <v>38</v>
-      </c>
-      <c r="D649" t="s">
-        <v>49</v>
-      </c>
-      <c r="E649" t="s">
-        <v>45</v>
-      </c>
-      <c r="F649" t="s">
-        <v>510</v>
-      </c>
-      <c r="G649" t="s">
-        <v>510</v>
-      </c>
-      <c r="H649" t="s">
-        <v>510</v>
-      </c>
-      <c r="I649" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="650">
-      <c r="B650" t="s">
-        <v>12187</v>
-      </c>
-      <c r="C650" t="s">
-        <v>38</v>
-      </c>
-      <c r="D650" t="s">
-        <v>49</v>
-      </c>
-      <c r="E650" t="s">
-        <v>45</v>
-      </c>
-      <c r="F650" t="s">
-        <v>512</v>
-      </c>
-      <c r="G650" t="s">
-        <v>512</v>
-      </c>
-      <c r="H650" t="s">
-        <v>512</v>
-      </c>
-      <c r="I650" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="651">
-      <c r="B651" t="s">
-        <v>12188</v>
-      </c>
-      <c r="C651" t="s">
-        <v>38</v>
-      </c>
-      <c r="D651" t="s">
-        <v>49</v>
-      </c>
-      <c r="E651" t="s">
-        <v>45</v>
-      </c>
-      <c r="F651" t="s">
-        <v>514</v>
-      </c>
-      <c r="G651" t="s">
-        <v>514</v>
-      </c>
-      <c r="H651" t="s">
-        <v>514</v>
-      </c>
-      <c r="I651" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="652">
-      <c r="B652" t="s">
-        <v>12189</v>
-      </c>
-      <c r="C652" t="s">
-        <v>38</v>
-      </c>
-      <c r="D652" t="s">
-        <v>49</v>
-      </c>
-      <c r="E652" t="s">
-        <v>45</v>
-      </c>
-      <c r="F652" t="s">
-        <v>516</v>
-      </c>
-      <c r="G652" t="s">
-        <v>516</v>
-      </c>
-      <c r="H652" t="s">
-        <v>516</v>
-      </c>
-      <c r="I652" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="653">
-      <c r="B653" t="s">
-        <v>12190</v>
-      </c>
-      <c r="C653" t="s">
-        <v>38</v>
-      </c>
-      <c r="D653" t="s">
-        <v>49</v>
-      </c>
-      <c r="E653" t="s">
-        <v>45</v>
-      </c>
-      <c r="F653" t="s">
-        <v>522</v>
-      </c>
-      <c r="G653" t="s">
-        <v>522</v>
-      </c>
-      <c r="H653" t="s">
-        <v>522</v>
-      </c>
-      <c r="I653" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="654">
-      <c r="B654" t="s">
-        <v>12191</v>
-      </c>
-      <c r="C654" t="s">
-        <v>38</v>
-      </c>
-      <c r="D654" t="s">
-        <v>49</v>
-      </c>
-      <c r="E654" t="s">
-        <v>45</v>
-      </c>
-      <c r="F654" t="s">
-        <v>1278</v>
-      </c>
-      <c r="G654" t="s">
-        <v>1278</v>
-      </c>
-      <c r="H654" t="s">
-        <v>1278</v>
-      </c>
-      <c r="I654" t="s">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="655">
-      <c r="B655" t="s">
-        <v>12192</v>
-      </c>
-      <c r="C655" t="s">
-        <v>38</v>
-      </c>
-      <c r="D655" t="s">
-        <v>49</v>
-      </c>
-      <c r="E655" t="s">
-        <v>45</v>
-      </c>
-      <c r="F655" t="s">
-        <v>1279</v>
-      </c>
-      <c r="G655" t="s">
-        <v>1279</v>
-      </c>
-      <c r="H655" t="s">
-        <v>1279</v>
-      </c>
-      <c r="I655" t="s">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="656">
-      <c r="B656" t="s">
-        <v>12193</v>
-      </c>
-      <c r="C656" t="s">
-        <v>38</v>
-      </c>
-      <c r="D656" t="s">
-        <v>49</v>
-      </c>
-      <c r="E656" t="s">
-        <v>45</v>
-      </c>
-      <c r="F656" t="s">
-        <v>1280</v>
-      </c>
-      <c r="G656" t="s">
-        <v>1280</v>
-      </c>
-      <c r="H656" t="s">
-        <v>1280</v>
-      </c>
-      <c r="I656" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="657">
-      <c r="B657" t="s">
-        <v>12194</v>
-      </c>
-      <c r="C657" t="s">
-        <v>38</v>
-      </c>
-      <c r="D657" t="s">
-        <v>49</v>
-      </c>
-      <c r="E657" t="s">
-        <v>45</v>
-      </c>
-      <c r="F657" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G657" t="s">
-        <v>1281</v>
-      </c>
-      <c r="H657" t="s">
-        <v>1281</v>
-      </c>
-      <c r="I657" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="658">
-      <c r="B658" t="s">
-        <v>12195</v>
-      </c>
-      <c r="C658" t="s">
-        <v>101</v>
-      </c>
-      <c r="D658" t="s">
-        <v>49</v>
-      </c>
-      <c r="E658" t="s">
-        <v>45</v>
-      </c>
-      <c r="F658" t="s">
-        <v>313</v>
-      </c>
-      <c r="G658" t="s">
-        <v>313</v>
-      </c>
-      <c r="H658" t="s">
-        <v>313</v>
-      </c>
-      <c r="I658" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="659">
-      <c r="B659" t="s">
-        <v>12196</v>
-      </c>
-      <c r="C659" t="s">
-        <v>101</v>
-      </c>
-      <c r="D659" t="s">
-        <v>49</v>
-      </c>
-      <c r="E659" t="s">
-        <v>45</v>
-      </c>
-      <c r="F659" t="s">
-        <v>1631</v>
-      </c>
-      <c r="G659" t="s">
-        <v>1631</v>
-      </c>
-      <c r="H659" t="s">
-        <v>1631</v>
-      </c>
-      <c r="I659" t="s">
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="660">
-      <c r="B660" t="s">
-        <v>12197</v>
-      </c>
-      <c r="C660" t="s">
-        <v>38</v>
-      </c>
-      <c r="D660" t="s">
-        <v>49</v>
-      </c>
-      <c r="E660" t="s">
-        <v>45</v>
-      </c>
-      <c r="F660" t="s">
-        <v>50</v>
-      </c>
-      <c r="G660" t="s">
-        <v>50</v>
-      </c>
-      <c r="H660" t="s">
-        <v>50</v>
-      </c>
-      <c r="I660" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="661">
-      <c r="B661" t="s">
-        <v>12198</v>
-      </c>
-      <c r="C661" t="s">
-        <v>38</v>
-      </c>
-      <c r="D661" t="s">
-        <v>44</v>
-      </c>
-      <c r="E661" t="s">
-        <v>45</v>
-      </c>
-      <c r="F661" t="s">
-        <v>12203</v>
-      </c>
-      <c r="G661" t="s">
-        <v>52</v>
-      </c>
-      <c r="H661" t="s">
-        <v>52</v>
-      </c>
-      <c r="I661" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="662">
-      <c r="B662" t="s">
-        <v>12199</v>
-      </c>
-      <c r="C662" t="s">
-        <v>38</v>
-      </c>
-      <c r="D662" t="s">
-        <v>49</v>
-      </c>
-      <c r="E662" t="s">
-        <v>45</v>
-      </c>
-      <c r="F662" t="s">
-        <v>50</v>
-      </c>
-      <c r="G662" t="s">
-        <v>50</v>
-      </c>
-      <c r="H662" t="s">
-        <v>50</v>
-      </c>
-      <c r="I662" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="663">
-      <c r="B663" t="s">
-        <v>12200</v>
-      </c>
-      <c r="C663" t="s">
-        <v>38</v>
-      </c>
-      <c r="D663" t="s">
-        <v>44</v>
-      </c>
-      <c r="E663" t="s">
-        <v>45</v>
-      </c>
-      <c r="F663" t="s">
-        <v>12204</v>
-      </c>
-      <c r="G663" t="s">
-        <v>52</v>
-      </c>
-      <c r="H663" t="s">
-        <v>52</v>
-      </c>
-      <c r="I663" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    </row>
+    <row r="643"/>
+    <row r="644"/>
+    <row r="645"/>
+    <row r="646"/>
+    <row r="647"/>
+    <row r="648"/>
+    <row r="649"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
     <row r="664"/>
     <row r="665"/>
     <row r="666"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-07-25 21-45-31
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156502" uniqueCount="12240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6180553" uniqueCount="12250">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41517,6 +41517,36 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4063</t>
   </si>
 </sst>
 </file>
@@ -42783,13 +42813,13 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="J6" t="s">
         <v>46</v>
@@ -43027,13 +43057,13 @@
         <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="H12" t="s">
         <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="J12" t="s">
         <v>46</v>
@@ -43378,13 +43408,13 @@
         <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="H24" t="s">
         <v>46</v>
       </c>
       <c r="I24" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="J24" t="s">
         <v>46</v>
@@ -43407,13 +43437,13 @@
         <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="H25" t="s">
         <v>46</v>
       </c>
       <c r="I25" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="J25" t="s">
         <v>46</v>
@@ -43436,13 +43466,13 @@
         <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="H26" t="s">
         <v>46</v>
       </c>
       <c r="I26" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="J26" t="s">
         <v>46</v>
@@ -59991,13 +60021,13 @@
         <v>390</v>
       </c>
       <c r="G637" t="s">
-        <v>284</v>
+        <v>390</v>
       </c>
       <c r="H637" t="s">
-        <v>284</v>
+        <v>390</v>
       </c>
       <c r="I637" t="s">
-        <v>284</v>
+        <v>390</v>
       </c>
     </row>
     <row r="638">
@@ -60416,16 +60446,266 @@
         <v>11930</v>
       </c>
     </row>
-    <row r="654"/>
-    <row r="655"/>
-    <row r="656"/>
-    <row r="657"/>
-    <row r="658"/>
-    <row r="659"/>
-    <row r="660"/>
-    <row r="661"/>
-    <row r="662"/>
-    <row r="663"/>
+    <row r="654">
+      <c r="B654" t="s">
+        <v>12240</v>
+      </c>
+      <c r="C654" t="s">
+        <v>11926</v>
+      </c>
+      <c r="D654" t="s">
+        <v>49</v>
+      </c>
+      <c r="E654" t="s">
+        <v>45</v>
+      </c>
+      <c r="F654" t="s">
+        <v>50</v>
+      </c>
+      <c r="G654" t="s">
+        <v>50</v>
+      </c>
+      <c r="H654" t="s">
+        <v>50</v>
+      </c>
+      <c r="I654" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="B655" t="s">
+        <v>12241</v>
+      </c>
+      <c r="C655" t="s">
+        <v>11926</v>
+      </c>
+      <c r="D655" t="s">
+        <v>44</v>
+      </c>
+      <c r="E655" t="s">
+        <v>45</v>
+      </c>
+      <c r="F655" t="s">
+        <v>11930</v>
+      </c>
+      <c r="G655" t="s">
+        <v>11930</v>
+      </c>
+      <c r="H655" t="s">
+        <v>11930</v>
+      </c>
+      <c r="I655" t="s">
+        <v>11930</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="B656" t="s">
+        <v>12242</v>
+      </c>
+      <c r="C656" t="s">
+        <v>38</v>
+      </c>
+      <c r="D656" t="s">
+        <v>49</v>
+      </c>
+      <c r="E656" t="s">
+        <v>45</v>
+      </c>
+      <c r="F656" t="s">
+        <v>50</v>
+      </c>
+      <c r="G656" t="s">
+        <v>50</v>
+      </c>
+      <c r="H656" t="s">
+        <v>50</v>
+      </c>
+      <c r="I656" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="B657" t="s">
+        <v>12243</v>
+      </c>
+      <c r="C657" t="s">
+        <v>38</v>
+      </c>
+      <c r="D657" t="s">
+        <v>44</v>
+      </c>
+      <c r="E657" t="s">
+        <v>45</v>
+      </c>
+      <c r="F657" t="s">
+        <v>390</v>
+      </c>
+      <c r="G657" t="s">
+        <v>390</v>
+      </c>
+      <c r="H657" t="s">
+        <v>390</v>
+      </c>
+      <c r="I657" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="B658" t="s">
+        <v>12244</v>
+      </c>
+      <c r="C658" t="s">
+        <v>38</v>
+      </c>
+      <c r="D658" t="s">
+        <v>49</v>
+      </c>
+      <c r="E658" t="s">
+        <v>45</v>
+      </c>
+      <c r="F658" t="s">
+        <v>50</v>
+      </c>
+      <c r="G658" t="s">
+        <v>50</v>
+      </c>
+      <c r="H658" t="s">
+        <v>50</v>
+      </c>
+      <c r="I658" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="B659" t="s">
+        <v>12245</v>
+      </c>
+      <c r="C659" t="s">
+        <v>38</v>
+      </c>
+      <c r="D659" t="s">
+        <v>44</v>
+      </c>
+      <c r="E659" t="s">
+        <v>45</v>
+      </c>
+      <c r="F659" t="s">
+        <v>390</v>
+      </c>
+      <c r="G659" t="s">
+        <v>390</v>
+      </c>
+      <c r="H659" t="s">
+        <v>390</v>
+      </c>
+      <c r="I659" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="B660" t="s">
+        <v>12246</v>
+      </c>
+      <c r="C660" t="s">
+        <v>38</v>
+      </c>
+      <c r="D660" t="s">
+        <v>49</v>
+      </c>
+      <c r="E660" t="s">
+        <v>45</v>
+      </c>
+      <c r="F660" t="s">
+        <v>50</v>
+      </c>
+      <c r="G660" t="s">
+        <v>50</v>
+      </c>
+      <c r="H660" t="s">
+        <v>50</v>
+      </c>
+      <c r="I660" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="B661" t="s">
+        <v>12247</v>
+      </c>
+      <c r="C661" t="s">
+        <v>38</v>
+      </c>
+      <c r="D661" t="s">
+        <v>44</v>
+      </c>
+      <c r="E661" t="s">
+        <v>45</v>
+      </c>
+      <c r="F661" t="s">
+        <v>390</v>
+      </c>
+      <c r="G661" t="s">
+        <v>390</v>
+      </c>
+      <c r="H661" t="s">
+        <v>390</v>
+      </c>
+      <c r="I661" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="B662" t="s">
+        <v>12248</v>
+      </c>
+      <c r="C662" t="s">
+        <v>38</v>
+      </c>
+      <c r="D662" t="s">
+        <v>49</v>
+      </c>
+      <c r="E662" t="s">
+        <v>45</v>
+      </c>
+      <c r="F662" t="s">
+        <v>50</v>
+      </c>
+      <c r="G662" t="s">
+        <v>50</v>
+      </c>
+      <c r="H662" t="s">
+        <v>50</v>
+      </c>
+      <c r="I662" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="B663" t="s">
+        <v>12249</v>
+      </c>
+      <c r="C663" t="s">
+        <v>38</v>
+      </c>
+      <c r="D663" t="s">
+        <v>44</v>
+      </c>
+      <c r="E663" t="s">
+        <v>45</v>
+      </c>
+      <c r="F663" t="s">
+        <v>390</v>
+      </c>
+      <c r="G663" t="s">
+        <v>390</v>
+      </c>
+      <c r="H663" t="s">
+        <v>390</v>
+      </c>
+      <c r="I663" t="s">
+        <v>390</v>
+      </c>
+    </row>
     <row r="664"/>
     <row r="665"/>
     <row r="666"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-08-01 21-42-09
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6180553" uniqueCount="12250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6214397" uniqueCount="12285">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41547,6 +41547,111 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?123</t>
   </si>
 </sst>
 </file>
@@ -60500,13 +60605,13 @@
     </row>
     <row r="656">
       <c r="B656" t="s">
-        <v>12242</v>
+        <v>12250</v>
       </c>
       <c r="C656" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D656" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E656" t="s">
         <v>45</v>
@@ -60526,33 +60631,33 @@
     </row>
     <row r="657">
       <c r="B657" t="s">
-        <v>12243</v>
+        <v>12251</v>
       </c>
       <c r="C657" t="s">
         <v>38</v>
       </c>
       <c r="D657" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E657" t="s">
         <v>45</v>
       </c>
       <c r="F657" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="G657" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="H657" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="I657" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
     </row>
     <row r="658">
       <c r="B658" t="s">
-        <v>12244</v>
+        <v>12252</v>
       </c>
       <c r="C658" t="s">
         <v>38</v>
@@ -60564,47 +60669,47 @@
         <v>45</v>
       </c>
       <c r="F658" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="G658" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="H658" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="I658" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
     </row>
     <row r="659">
       <c r="B659" t="s">
-        <v>12245</v>
+        <v>12253</v>
       </c>
       <c r="C659" t="s">
         <v>38</v>
       </c>
       <c r="D659" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E659" t="s">
         <v>45</v>
       </c>
       <c r="F659" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="G659" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="H659" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="I659" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
     </row>
     <row r="660">
       <c r="B660" t="s">
-        <v>12246</v>
+        <v>12254</v>
       </c>
       <c r="C660" t="s">
         <v>38</v>
@@ -60616,47 +60721,47 @@
         <v>45</v>
       </c>
       <c r="F660" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="G660" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="H660" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="I660" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
     </row>
     <row r="661">
       <c r="B661" t="s">
-        <v>12247</v>
+        <v>12255</v>
       </c>
       <c r="C661" t="s">
         <v>38</v>
       </c>
       <c r="D661" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E661" t="s">
         <v>45</v>
       </c>
       <c r="F661" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="G661" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="H661" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
       <c r="I661" t="s">
-        <v>390</v>
+        <v>235</v>
       </c>
     </row>
     <row r="662">
       <c r="B662" t="s">
-        <v>12248</v>
+        <v>12256</v>
       </c>
       <c r="C662" t="s">
         <v>38</v>
@@ -60668,69 +60773,694 @@
         <v>45</v>
       </c>
       <c r="F662" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="G662" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="H662" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="I662" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
     </row>
     <row r="663">
       <c r="B663" t="s">
-        <v>12249</v>
+        <v>12257</v>
       </c>
       <c r="C663" t="s">
         <v>38</v>
       </c>
       <c r="D663" t="s">
+        <v>49</v>
+      </c>
+      <c r="E663" t="s">
+        <v>45</v>
+      </c>
+      <c r="F663" t="s">
+        <v>235</v>
+      </c>
+      <c r="G663" t="s">
+        <v>235</v>
+      </c>
+      <c r="H663" t="s">
+        <v>235</v>
+      </c>
+      <c r="I663" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="B664" t="s">
+        <v>12258</v>
+      </c>
+      <c r="C664" t="s">
+        <v>38</v>
+      </c>
+      <c r="D664" t="s">
+        <v>49</v>
+      </c>
+      <c r="E664" t="s">
+        <v>45</v>
+      </c>
+      <c r="F664" t="s">
+        <v>235</v>
+      </c>
+      <c r="G664" t="s">
+        <v>235</v>
+      </c>
+      <c r="H664" t="s">
+        <v>235</v>
+      </c>
+      <c r="I664" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="B665" t="s">
+        <v>12259</v>
+      </c>
+      <c r="C665" t="s">
+        <v>38</v>
+      </c>
+      <c r="D665" t="s">
+        <v>49</v>
+      </c>
+      <c r="E665" t="s">
+        <v>45</v>
+      </c>
+      <c r="F665" t="s">
+        <v>235</v>
+      </c>
+      <c r="G665" t="s">
+        <v>235</v>
+      </c>
+      <c r="H665" t="s">
+        <v>235</v>
+      </c>
+      <c r="I665" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="B666" t="s">
+        <v>12260</v>
+      </c>
+      <c r="C666" t="s">
+        <v>38</v>
+      </c>
+      <c r="D666" t="s">
+        <v>49</v>
+      </c>
+      <c r="E666" t="s">
+        <v>45</v>
+      </c>
+      <c r="F666" t="s">
+        <v>235</v>
+      </c>
+      <c r="G666" t="s">
+        <v>235</v>
+      </c>
+      <c r="H666" t="s">
+        <v>235</v>
+      </c>
+      <c r="I666" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="B667" t="s">
+        <v>12261</v>
+      </c>
+      <c r="C667" t="s">
+        <v>38</v>
+      </c>
+      <c r="D667" t="s">
         <v>44</v>
       </c>
-      <c r="E663" t="s">
-        <v>45</v>
-      </c>
-      <c r="F663" t="s">
-        <v>390</v>
-      </c>
-      <c r="G663" t="s">
-        <v>390</v>
-      </c>
-      <c r="H663" t="s">
-        <v>390</v>
-      </c>
-      <c r="I663" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="664"/>
-    <row r="665"/>
-    <row r="666"/>
-    <row r="667"/>
-    <row r="668"/>
-    <row r="669"/>
-    <row r="670"/>
-    <row r="671"/>
-    <row r="672"/>
-    <row r="673"/>
-    <row r="674"/>
-    <row r="675"/>
-    <row r="676"/>
-    <row r="677"/>
-    <row r="678"/>
-    <row r="679"/>
-    <row r="680"/>
-    <row r="681"/>
-    <row r="682"/>
-    <row r="683"/>
-    <row r="684"/>
-    <row r="685"/>
-    <row r="686"/>
-    <row r="687"/>
-    <row r="688"/>
+      <c r="E667" t="s">
+        <v>45</v>
+      </c>
+      <c r="F667" t="s">
+        <v>235</v>
+      </c>
+      <c r="G667" t="s">
+        <v>235</v>
+      </c>
+      <c r="H667" t="s">
+        <v>235</v>
+      </c>
+      <c r="I667" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="B668" t="s">
+        <v>12262</v>
+      </c>
+      <c r="C668" t="s">
+        <v>38</v>
+      </c>
+      <c r="D668" t="s">
+        <v>44</v>
+      </c>
+      <c r="E668" t="s">
+        <v>45</v>
+      </c>
+      <c r="F668" t="s">
+        <v>235</v>
+      </c>
+      <c r="G668" t="s">
+        <v>235</v>
+      </c>
+      <c r="H668" t="s">
+        <v>235</v>
+      </c>
+      <c r="I668" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="B669" t="s">
+        <v>12263</v>
+      </c>
+      <c r="C669" t="s">
+        <v>38</v>
+      </c>
+      <c r="D669" t="s">
+        <v>44</v>
+      </c>
+      <c r="E669" t="s">
+        <v>45</v>
+      </c>
+      <c r="F669" t="s">
+        <v>235</v>
+      </c>
+      <c r="G669" t="s">
+        <v>235</v>
+      </c>
+      <c r="H669" t="s">
+        <v>235</v>
+      </c>
+      <c r="I669" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="B670" t="s">
+        <v>12264</v>
+      </c>
+      <c r="C670" t="s">
+        <v>38</v>
+      </c>
+      <c r="D670" t="s">
+        <v>44</v>
+      </c>
+      <c r="E670" t="s">
+        <v>45</v>
+      </c>
+      <c r="F670" t="s">
+        <v>235</v>
+      </c>
+      <c r="G670" t="s">
+        <v>235</v>
+      </c>
+      <c r="H670" t="s">
+        <v>235</v>
+      </c>
+      <c r="I670" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="B671" t="s">
+        <v>12265</v>
+      </c>
+      <c r="C671" t="s">
+        <v>38</v>
+      </c>
+      <c r="D671" t="s">
+        <v>44</v>
+      </c>
+      <c r="E671" t="s">
+        <v>45</v>
+      </c>
+      <c r="F671" t="s">
+        <v>235</v>
+      </c>
+      <c r="G671" t="s">
+        <v>235</v>
+      </c>
+      <c r="H671" t="s">
+        <v>235</v>
+      </c>
+      <c r="I671" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="B672" t="s">
+        <v>12266</v>
+      </c>
+      <c r="C672" t="s">
+        <v>38</v>
+      </c>
+      <c r="D672" t="s">
+        <v>44</v>
+      </c>
+      <c r="E672" t="s">
+        <v>45</v>
+      </c>
+      <c r="F672" t="s">
+        <v>235</v>
+      </c>
+      <c r="G672" t="s">
+        <v>235</v>
+      </c>
+      <c r="H672" t="s">
+        <v>235</v>
+      </c>
+      <c r="I672" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="B673" t="s">
+        <v>12267</v>
+      </c>
+      <c r="C673" t="s">
+        <v>38</v>
+      </c>
+      <c r="D673" t="s">
+        <v>44</v>
+      </c>
+      <c r="E673" t="s">
+        <v>45</v>
+      </c>
+      <c r="F673" t="s">
+        <v>235</v>
+      </c>
+      <c r="G673" t="s">
+        <v>235</v>
+      </c>
+      <c r="H673" t="s">
+        <v>235</v>
+      </c>
+      <c r="I673" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="B674" t="s">
+        <v>12268</v>
+      </c>
+      <c r="C674" t="s">
+        <v>38</v>
+      </c>
+      <c r="D674" t="s">
+        <v>44</v>
+      </c>
+      <c r="E674" t="s">
+        <v>45</v>
+      </c>
+      <c r="F674" t="s">
+        <v>235</v>
+      </c>
+      <c r="G674" t="s">
+        <v>235</v>
+      </c>
+      <c r="H674" t="s">
+        <v>235</v>
+      </c>
+      <c r="I674" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="B675" t="s">
+        <v>12269</v>
+      </c>
+      <c r="C675" t="s">
+        <v>38</v>
+      </c>
+      <c r="D675" t="s">
+        <v>44</v>
+      </c>
+      <c r="E675" t="s">
+        <v>45</v>
+      </c>
+      <c r="F675" t="s">
+        <v>235</v>
+      </c>
+      <c r="G675" t="s">
+        <v>235</v>
+      </c>
+      <c r="H675" t="s">
+        <v>235</v>
+      </c>
+      <c r="I675" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="B676" t="s">
+        <v>12270</v>
+      </c>
+      <c r="C676" t="s">
+        <v>38</v>
+      </c>
+      <c r="D676" t="s">
+        <v>44</v>
+      </c>
+      <c r="E676" t="s">
+        <v>45</v>
+      </c>
+      <c r="F676" t="s">
+        <v>235</v>
+      </c>
+      <c r="G676" t="s">
+        <v>235</v>
+      </c>
+      <c r="H676" t="s">
+        <v>235</v>
+      </c>
+      <c r="I676" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="B677" t="s">
+        <v>12271</v>
+      </c>
+      <c r="C677" t="s">
+        <v>38</v>
+      </c>
+      <c r="D677" t="s">
+        <v>44</v>
+      </c>
+      <c r="E677" t="s">
+        <v>45</v>
+      </c>
+      <c r="F677" t="s">
+        <v>235</v>
+      </c>
+      <c r="G677" t="s">
+        <v>235</v>
+      </c>
+      <c r="H677" t="s">
+        <v>235</v>
+      </c>
+      <c r="I677" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="B678" t="s">
+        <v>12272</v>
+      </c>
+      <c r="C678" t="s">
+        <v>38</v>
+      </c>
+      <c r="D678" t="s">
+        <v>44</v>
+      </c>
+      <c r="E678" t="s">
+        <v>45</v>
+      </c>
+      <c r="F678" t="s">
+        <v>235</v>
+      </c>
+      <c r="G678" t="s">
+        <v>235</v>
+      </c>
+      <c r="H678" t="s">
+        <v>235</v>
+      </c>
+      <c r="I678" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="B679" t="s">
+        <v>12273</v>
+      </c>
+      <c r="C679" t="s">
+        <v>38</v>
+      </c>
+      <c r="D679" t="s">
+        <v>44</v>
+      </c>
+      <c r="E679" t="s">
+        <v>45</v>
+      </c>
+      <c r="F679" t="s">
+        <v>235</v>
+      </c>
+      <c r="G679" t="s">
+        <v>235</v>
+      </c>
+      <c r="H679" t="s">
+        <v>235</v>
+      </c>
+      <c r="I679" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="B680" t="s">
+        <v>12274</v>
+      </c>
+      <c r="C680" t="s">
+        <v>38</v>
+      </c>
+      <c r="D680" t="s">
+        <v>44</v>
+      </c>
+      <c r="E680" t="s">
+        <v>45</v>
+      </c>
+      <c r="F680" t="s">
+        <v>235</v>
+      </c>
+      <c r="G680" t="s">
+        <v>235</v>
+      </c>
+      <c r="H680" t="s">
+        <v>235</v>
+      </c>
+      <c r="I680" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="B681" t="s">
+        <v>12275</v>
+      </c>
+      <c r="C681" t="s">
+        <v>38</v>
+      </c>
+      <c r="D681" t="s">
+        <v>44</v>
+      </c>
+      <c r="E681" t="s">
+        <v>45</v>
+      </c>
+      <c r="F681" t="s">
+        <v>235</v>
+      </c>
+      <c r="G681" t="s">
+        <v>235</v>
+      </c>
+      <c r="H681" t="s">
+        <v>235</v>
+      </c>
+      <c r="I681" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="B682" t="s">
+        <v>12276</v>
+      </c>
+      <c r="C682" t="s">
+        <v>38</v>
+      </c>
+      <c r="D682" t="s">
+        <v>44</v>
+      </c>
+      <c r="E682" t="s">
+        <v>45</v>
+      </c>
+      <c r="F682" t="s">
+        <v>235</v>
+      </c>
+      <c r="G682" t="s">
+        <v>235</v>
+      </c>
+      <c r="H682" t="s">
+        <v>235</v>
+      </c>
+      <c r="I682" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="B683" t="s">
+        <v>12277</v>
+      </c>
+      <c r="C683" t="s">
+        <v>38</v>
+      </c>
+      <c r="D683" t="s">
+        <v>44</v>
+      </c>
+      <c r="E683" t="s">
+        <v>45</v>
+      </c>
+      <c r="F683" t="s">
+        <v>235</v>
+      </c>
+      <c r="G683" t="s">
+        <v>235</v>
+      </c>
+      <c r="H683" t="s">
+        <v>235</v>
+      </c>
+      <c r="I683" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="B684" t="s">
+        <v>12278</v>
+      </c>
+      <c r="C684" t="s">
+        <v>38</v>
+      </c>
+      <c r="D684" t="s">
+        <v>44</v>
+      </c>
+      <c r="E684" t="s">
+        <v>45</v>
+      </c>
+      <c r="F684" t="s">
+        <v>235</v>
+      </c>
+      <c r="G684" t="s">
+        <v>235</v>
+      </c>
+      <c r="H684" t="s">
+        <v>235</v>
+      </c>
+      <c r="I684" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="B685" t="s">
+        <v>12279</v>
+      </c>
+      <c r="C685" t="s">
+        <v>38</v>
+      </c>
+      <c r="D685" t="s">
+        <v>44</v>
+      </c>
+      <c r="E685" t="s">
+        <v>45</v>
+      </c>
+      <c r="F685" t="s">
+        <v>235</v>
+      </c>
+      <c r="G685" t="s">
+        <v>235</v>
+      </c>
+      <c r="H685" t="s">
+        <v>235</v>
+      </c>
+      <c r="I685" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="B686" t="s">
+        <v>12280</v>
+      </c>
+      <c r="C686" t="s">
+        <v>41</v>
+      </c>
+      <c r="D686" t="s">
+        <v>49</v>
+      </c>
+      <c r="E686" t="s">
+        <v>45</v>
+      </c>
+      <c r="F686" t="s">
+        <v>241</v>
+      </c>
+      <c r="G686" t="s">
+        <v>241</v>
+      </c>
+      <c r="H686" t="s">
+        <v>241</v>
+      </c>
+      <c r="I686" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="B687" t="s">
+        <v>12281</v>
+      </c>
+      <c r="C687" t="s">
+        <v>41</v>
+      </c>
+      <c r="D687" t="s">
+        <v>49</v>
+      </c>
+      <c r="E687" t="s">
+        <v>45</v>
+      </c>
+      <c r="F687" t="s">
+        <v>238</v>
+      </c>
+      <c r="G687" t="s">
+        <v>238</v>
+      </c>
+      <c r="H687" t="s">
+        <v>238</v>
+      </c>
+      <c r="I687" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="B688" t="s">
+        <v>12283</v>
+      </c>
+      <c r="C688" t="s">
+        <v>41</v>
+      </c>
+      <c r="D688" t="s">
+        <v>49</v>
+      </c>
+      <c r="E688" t="s">
+        <v>45</v>
+      </c>
+      <c r="F688" t="s">
+        <v>12284</v>
+      </c>
+      <c r="G688" t="s">
+        <v>12284</v>
+      </c>
+      <c r="H688" t="s">
+        <v>12284</v>
+      </c>
+      <c r="I688" t="s">
+        <v>12284</v>
+      </c>
+    </row>
     <row r="689"/>
     <row r="690"/>
     <row r="691"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-08-02 21-37-19
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6214397" uniqueCount="12285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6239612" uniqueCount="12287">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41652,6 +41652,12 @@
   </si>
   <si>
     <t xml:space="preserve">?123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4099</t>
   </si>
 </sst>
 </file>
@@ -61461,8 +61467,58 @@
         <v>12284</v>
       </c>
     </row>
-    <row r="689"/>
-    <row r="690"/>
+    <row r="689">
+      <c r="B689" t="s">
+        <v>12285</v>
+      </c>
+      <c r="C689" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D689" t="s">
+        <v>44</v>
+      </c>
+      <c r="E689" t="s">
+        <v>45</v>
+      </c>
+      <c r="F689" t="s">
+        <v>1294</v>
+      </c>
+      <c r="G689" t="s">
+        <v>1294</v>
+      </c>
+      <c r="H689" t="s">
+        <v>1294</v>
+      </c>
+      <c r="I689" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="B690" t="s">
+        <v>12286</v>
+      </c>
+      <c r="C690" t="s">
+        <v>78</v>
+      </c>
+      <c r="D690" t="s">
+        <v>44</v>
+      </c>
+      <c r="E690" t="s">
+        <v>45</v>
+      </c>
+      <c r="F690" t="s">
+        <v>1294</v>
+      </c>
+      <c r="G690" t="s">
+        <v>12048</v>
+      </c>
+      <c r="H690" t="s">
+        <v>12048</v>
+      </c>
+      <c r="I690" t="s">
+        <v>12048</v>
+      </c>
+    </row>
     <row r="691"/>
     <row r="692"/>
     <row r="693"/>

</xml_diff>

<commit_message>
Create the Timing Scrpts process
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6239612" uniqueCount="12287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6264908" uniqueCount="12293">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41658,6 +41658,24 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SegoeUI30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segoeui.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen1</t>
   </si>
 </sst>
 </file>
@@ -43586,6 +43604,35 @@
         <v>249</v>
       </c>
       <c r="J26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>12287</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12288</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
+        <v>250</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" t="s">
+        <v>249</v>
+      </c>
+      <c r="J27" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix Touch build issue 1
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6264908" uniqueCount="12293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273352" uniqueCount="12293">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -61566,8 +61566,58 @@
         <v>12048</v>
       </c>
     </row>
-    <row r="691"/>
-    <row r="692"/>
+    <row r="691">
+      <c r="B691" t="s">
+        <v>12289</v>
+      </c>
+      <c r="C691" t="s">
+        <v>38</v>
+      </c>
+      <c r="D691" t="s">
+        <v>44</v>
+      </c>
+      <c r="E691" t="s">
+        <v>45</v>
+      </c>
+      <c r="F691" t="s">
+        <v>47</v>
+      </c>
+      <c r="G691" t="s">
+        <v>47</v>
+      </c>
+      <c r="H691" t="s">
+        <v>47</v>
+      </c>
+      <c r="I691" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="B692" t="s">
+        <v>12291</v>
+      </c>
+      <c r="C692" t="s">
+        <v>38</v>
+      </c>
+      <c r="D692" t="s">
+        <v>44</v>
+      </c>
+      <c r="E692" t="s">
+        <v>45</v>
+      </c>
+      <c r="F692" t="s">
+        <v>47</v>
+      </c>
+      <c r="G692" t="s">
+        <v>47</v>
+      </c>
+      <c r="H692" t="s">
+        <v>47</v>
+      </c>
+      <c r="I692" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="693"/>
     <row r="694"/>
     <row r="695"/>

</xml_diff>

<commit_message>
Fixed file touch gfx
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273352" uniqueCount="12293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6281796" uniqueCount="12293">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -61606,16 +61606,16 @@
         <v>45</v>
       </c>
       <c r="F692" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G692" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H692" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I692" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="693"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-08-14 19-46-41
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6393212" uniqueCount="12363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439188" uniqueCount="12364">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41893,6 +41893,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4165</t>
   </si>
 </sst>
 </file>
@@ -59627,36 +59630,36 @@
     </row>
     <row r="608">
       <c r="B608" t="s">
-        <v>12101</v>
+        <v>12104</v>
       </c>
       <c r="C608" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D608" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E608" t="s">
         <v>45</v>
       </c>
       <c r="F608" t="s">
-        <v>12102</v>
+        <v>1574</v>
       </c>
       <c r="G608" t="s">
-        <v>12102</v>
+        <v>1574</v>
       </c>
       <c r="H608" t="s">
-        <v>12102</v>
+        <v>1574</v>
       </c>
       <c r="I608" t="s">
-        <v>12102</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="609">
       <c r="B609" t="s">
-        <v>12104</v>
+        <v>12105</v>
       </c>
       <c r="C609" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D609" t="s">
         <v>44</v>
@@ -59665,24 +59668,24 @@
         <v>45</v>
       </c>
       <c r="F609" t="s">
-        <v>1574</v>
+        <v>11458</v>
       </c>
       <c r="G609" t="s">
-        <v>1574</v>
+        <v>11458</v>
       </c>
       <c r="H609" t="s">
-        <v>1574</v>
+        <v>11458</v>
       </c>
       <c r="I609" t="s">
-        <v>1574</v>
+        <v>11458</v>
       </c>
     </row>
     <row r="610">
       <c r="B610" t="s">
-        <v>12105</v>
+        <v>12106</v>
       </c>
       <c r="C610" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D610" t="s">
         <v>44</v>
@@ -59691,76 +59694,76 @@
         <v>45</v>
       </c>
       <c r="F610" t="s">
-        <v>11458</v>
+        <v>11462</v>
       </c>
       <c r="G610" t="s">
-        <v>11458</v>
+        <v>11462</v>
       </c>
       <c r="H610" t="s">
-        <v>11458</v>
+        <v>11462</v>
       </c>
       <c r="I610" t="s">
-        <v>11458</v>
+        <v>11462</v>
       </c>
     </row>
     <row r="611">
       <c r="B611" t="s">
-        <v>12106</v>
+        <v>12107</v>
       </c>
       <c r="C611" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D611" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E611" t="s">
         <v>45</v>
       </c>
       <c r="F611" t="s">
-        <v>11462</v>
+        <v>50</v>
       </c>
       <c r="G611" t="s">
-        <v>11462</v>
+        <v>50</v>
       </c>
       <c r="H611" t="s">
-        <v>11462</v>
+        <v>50</v>
       </c>
       <c r="I611" t="s">
-        <v>11462</v>
+        <v>50</v>
       </c>
     </row>
     <row r="612">
       <c r="B612" t="s">
-        <v>12107</v>
+        <v>12108</v>
       </c>
       <c r="C612" t="s">
         <v>77</v>
       </c>
       <c r="D612" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E612" t="s">
         <v>45</v>
       </c>
       <c r="F612" t="s">
-        <v>50</v>
+        <v>11512</v>
       </c>
       <c r="G612" t="s">
-        <v>50</v>
+        <v>11512</v>
       </c>
       <c r="H612" t="s">
-        <v>50</v>
+        <v>11512</v>
       </c>
       <c r="I612" t="s">
-        <v>50</v>
+        <v>11512</v>
       </c>
     </row>
     <row r="613">
       <c r="B613" t="s">
-        <v>12108</v>
+        <v>12109</v>
       </c>
       <c r="C613" t="s">
-        <v>77</v>
+        <v>11926</v>
       </c>
       <c r="D613" t="s">
         <v>44</v>
@@ -59769,99 +59772,99 @@
         <v>45</v>
       </c>
       <c r="F613" t="s">
-        <v>11512</v>
+        <v>11930</v>
       </c>
       <c r="G613" t="s">
-        <v>11512</v>
+        <v>47</v>
       </c>
       <c r="H613" t="s">
-        <v>11512</v>
+        <v>47</v>
       </c>
       <c r="I613" t="s">
-        <v>11512</v>
+        <v>47</v>
       </c>
     </row>
     <row r="614">
       <c r="B614" t="s">
-        <v>12109</v>
+        <v>12110</v>
       </c>
       <c r="C614" t="s">
-        <v>11926</v>
+        <v>101</v>
       </c>
       <c r="D614" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E614" t="s">
         <v>45</v>
       </c>
       <c r="F614" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="G614" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H614" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I614" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="615">
       <c r="B615" t="s">
-        <v>12110</v>
+        <v>12111</v>
       </c>
       <c r="C615" t="s">
         <v>101</v>
       </c>
       <c r="D615" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E615" t="s">
         <v>45</v>
       </c>
       <c r="F615" t="s">
-        <v>50</v>
+        <v>11510</v>
       </c>
       <c r="G615" t="s">
-        <v>50</v>
+        <v>11510</v>
       </c>
       <c r="H615" t="s">
-        <v>50</v>
+        <v>11510</v>
       </c>
       <c r="I615" t="s">
-        <v>50</v>
+        <v>11510</v>
       </c>
     </row>
     <row r="616">
       <c r="B616" t="s">
-        <v>12111</v>
+        <v>12114</v>
       </c>
       <c r="C616" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D616" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E616" t="s">
         <v>45</v>
       </c>
       <c r="F616" t="s">
-        <v>11510</v>
+        <v>2570</v>
       </c>
       <c r="G616" t="s">
-        <v>11510</v>
+        <v>2570</v>
       </c>
       <c r="H616" t="s">
-        <v>11510</v>
+        <v>2570</v>
       </c>
       <c r="I616" t="s">
-        <v>11510</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="617">
       <c r="B617" t="s">
-        <v>12114</v>
+        <v>12115</v>
       </c>
       <c r="C617" t="s">
         <v>77</v>
@@ -59873,21 +59876,21 @@
         <v>45</v>
       </c>
       <c r="F617" t="s">
-        <v>2570</v>
+        <v>2574</v>
       </c>
       <c r="G617" t="s">
-        <v>2570</v>
+        <v>2574</v>
       </c>
       <c r="H617" t="s">
-        <v>2570</v>
+        <v>2574</v>
       </c>
       <c r="I617" t="s">
-        <v>2570</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="618">
       <c r="B618" t="s">
-        <v>12115</v>
+        <v>12116</v>
       </c>
       <c r="C618" t="s">
         <v>77</v>
@@ -59899,21 +59902,21 @@
         <v>45</v>
       </c>
       <c r="F618" t="s">
-        <v>2574</v>
+        <v>12117</v>
       </c>
       <c r="G618" t="s">
-        <v>2574</v>
+        <v>12117</v>
       </c>
       <c r="H618" t="s">
-        <v>2574</v>
+        <v>12117</v>
       </c>
       <c r="I618" t="s">
-        <v>2574</v>
+        <v>12117</v>
       </c>
     </row>
     <row r="619">
       <c r="B619" t="s">
-        <v>12116</v>
+        <v>12120</v>
       </c>
       <c r="C619" t="s">
         <v>77</v>
@@ -59925,21 +59928,21 @@
         <v>45</v>
       </c>
       <c r="F619" t="s">
-        <v>12117</v>
+        <v>2574</v>
       </c>
       <c r="G619" t="s">
-        <v>12117</v>
+        <v>2574</v>
       </c>
       <c r="H619" t="s">
-        <v>12117</v>
+        <v>2574</v>
       </c>
       <c r="I619" t="s">
-        <v>12117</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="620">
       <c r="B620" t="s">
-        <v>12120</v>
+        <v>12121</v>
       </c>
       <c r="C620" t="s">
         <v>77</v>
@@ -59951,21 +59954,21 @@
         <v>45</v>
       </c>
       <c r="F620" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="G620" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="H620" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="I620" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="621">
       <c r="B621" t="s">
-        <v>12121</v>
+        <v>12122</v>
       </c>
       <c r="C621" t="s">
         <v>77</v>
@@ -59977,24 +59980,24 @@
         <v>45</v>
       </c>
       <c r="F621" t="s">
-        <v>2570</v>
+        <v>12123</v>
       </c>
       <c r="G621" t="s">
-        <v>2570</v>
+        <v>12123</v>
       </c>
       <c r="H621" t="s">
-        <v>2570</v>
+        <v>12123</v>
       </c>
       <c r="I621" t="s">
-        <v>2570</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="622">
       <c r="B622" t="s">
-        <v>12122</v>
+        <v>12124</v>
       </c>
       <c r="C622" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D622" t="s">
         <v>49</v>
@@ -60003,21 +60006,21 @@
         <v>45</v>
       </c>
       <c r="F622" t="s">
-        <v>12123</v>
+        <v>2450</v>
       </c>
       <c r="G622" t="s">
-        <v>12123</v>
+        <v>2450</v>
       </c>
       <c r="H622" t="s">
-        <v>12123</v>
+        <v>2450</v>
       </c>
       <c r="I622" t="s">
-        <v>12123</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="623">
       <c r="B623" t="s">
-        <v>12124</v>
+        <v>12125</v>
       </c>
       <c r="C623" t="s">
         <v>78</v>
@@ -60029,24 +60032,24 @@
         <v>45</v>
       </c>
       <c r="F623" t="s">
-        <v>2450</v>
+        <v>12126</v>
       </c>
       <c r="G623" t="s">
-        <v>2450</v>
+        <v>12126</v>
       </c>
       <c r="H623" t="s">
-        <v>2450</v>
+        <v>12126</v>
       </c>
       <c r="I623" t="s">
-        <v>2450</v>
+        <v>12126</v>
       </c>
     </row>
     <row r="624">
       <c r="B624" t="s">
-        <v>12125</v>
+        <v>12127</v>
       </c>
       <c r="C624" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D624" t="s">
         <v>49</v>
@@ -60055,24 +60058,24 @@
         <v>45</v>
       </c>
       <c r="F624" t="s">
-        <v>12126</v>
+        <v>12128</v>
       </c>
       <c r="G624" t="s">
-        <v>12126</v>
+        <v>12128</v>
       </c>
       <c r="H624" t="s">
-        <v>12126</v>
+        <v>12128</v>
       </c>
       <c r="I624" t="s">
-        <v>12126</v>
+        <v>12128</v>
       </c>
     </row>
     <row r="625">
       <c r="B625" t="s">
-        <v>12127</v>
+        <v>12129</v>
       </c>
       <c r="C625" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D625" t="s">
         <v>49</v>
@@ -60081,73 +60084,73 @@
         <v>45</v>
       </c>
       <c r="F625" t="s">
-        <v>12128</v>
+        <v>50</v>
       </c>
       <c r="G625" t="s">
-        <v>12128</v>
+        <v>50</v>
       </c>
       <c r="H625" t="s">
-        <v>12128</v>
+        <v>50</v>
       </c>
       <c r="I625" t="s">
-        <v>12128</v>
+        <v>50</v>
       </c>
     </row>
     <row r="626">
       <c r="B626" t="s">
-        <v>12129</v>
+        <v>12130</v>
       </c>
       <c r="C626" t="s">
         <v>78</v>
       </c>
       <c r="D626" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E626" t="s">
         <v>45</v>
       </c>
       <c r="F626" t="s">
-        <v>50</v>
+        <v>12131</v>
       </c>
       <c r="G626" t="s">
-        <v>50</v>
+        <v>12131</v>
       </c>
       <c r="H626" t="s">
-        <v>50</v>
+        <v>12131</v>
       </c>
       <c r="I626" t="s">
-        <v>50</v>
+        <v>12131</v>
       </c>
     </row>
     <row r="627">
       <c r="B627" t="s">
-        <v>12130</v>
+        <v>12132</v>
       </c>
       <c r="C627" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D627" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E627" t="s">
         <v>45</v>
       </c>
       <c r="F627" t="s">
-        <v>12131</v>
+        <v>2574</v>
       </c>
       <c r="G627" t="s">
-        <v>12131</v>
+        <v>2574</v>
       </c>
       <c r="H627" t="s">
-        <v>12131</v>
+        <v>2574</v>
       </c>
       <c r="I627" t="s">
-        <v>12131</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="628">
       <c r="B628" t="s">
-        <v>12132</v>
+        <v>12133</v>
       </c>
       <c r="C628" t="s">
         <v>77</v>
@@ -60159,21 +60162,21 @@
         <v>45</v>
       </c>
       <c r="F628" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="G628" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="H628" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="I628" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="629">
       <c r="B629" t="s">
-        <v>12133</v>
+        <v>12134</v>
       </c>
       <c r="C629" t="s">
         <v>77</v>
@@ -60185,21 +60188,21 @@
         <v>45</v>
       </c>
       <c r="F629" t="s">
-        <v>2570</v>
+        <v>12135</v>
       </c>
       <c r="G629" t="s">
-        <v>2570</v>
+        <v>12135</v>
       </c>
       <c r="H629" t="s">
-        <v>2570</v>
+        <v>12135</v>
       </c>
       <c r="I629" t="s">
-        <v>2570</v>
+        <v>12135</v>
       </c>
     </row>
     <row r="630">
       <c r="B630" t="s">
-        <v>12134</v>
+        <v>12148</v>
       </c>
       <c r="C630" t="s">
         <v>77</v>
@@ -60211,50 +60214,50 @@
         <v>45</v>
       </c>
       <c r="F630" t="s">
-        <v>12135</v>
+        <v>50</v>
       </c>
       <c r="G630" t="s">
-        <v>12135</v>
+        <v>50</v>
       </c>
       <c r="H630" t="s">
-        <v>12135</v>
+        <v>50</v>
       </c>
       <c r="I630" t="s">
-        <v>12135</v>
+        <v>50</v>
       </c>
     </row>
     <row r="631">
       <c r="B631" t="s">
-        <v>12148</v>
+        <v>12149</v>
       </c>
       <c r="C631" t="s">
         <v>77</v>
       </c>
       <c r="D631" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E631" t="s">
         <v>45</v>
       </c>
       <c r="F631" t="s">
-        <v>50</v>
+        <v>11550</v>
       </c>
       <c r="G631" t="s">
-        <v>50</v>
+        <v>11550</v>
       </c>
       <c r="H631" t="s">
-        <v>50</v>
+        <v>11550</v>
       </c>
       <c r="I631" t="s">
-        <v>50</v>
+        <v>11550</v>
       </c>
     </row>
     <row r="632">
       <c r="B632" t="s">
-        <v>12149</v>
+        <v>12150</v>
       </c>
       <c r="C632" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D632" t="s">
         <v>44</v>
@@ -60263,21 +60266,21 @@
         <v>45</v>
       </c>
       <c r="F632" t="s">
-        <v>11550</v>
+        <v>12048</v>
       </c>
       <c r="G632" t="s">
-        <v>11550</v>
+        <v>12048</v>
       </c>
       <c r="H632" t="s">
-        <v>11550</v>
+        <v>12048</v>
       </c>
       <c r="I632" t="s">
-        <v>11550</v>
+        <v>12048</v>
       </c>
     </row>
     <row r="633">
       <c r="B633" t="s">
-        <v>12150</v>
+        <v>12151</v>
       </c>
       <c r="C633" t="s">
         <v>78</v>
@@ -60289,76 +60292,76 @@
         <v>45</v>
       </c>
       <c r="F633" t="s">
-        <v>12048</v>
+        <v>12152</v>
       </c>
       <c r="G633" t="s">
-        <v>12048</v>
+        <v>12152</v>
       </c>
       <c r="H633" t="s">
-        <v>12048</v>
+        <v>12152</v>
       </c>
       <c r="I633" t="s">
-        <v>12048</v>
+        <v>12152</v>
       </c>
     </row>
     <row r="634">
       <c r="B634" t="s">
-        <v>12151</v>
+        <v>12153</v>
       </c>
       <c r="C634" t="s">
         <v>78</v>
       </c>
       <c r="D634" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E634" t="s">
         <v>45</v>
       </c>
       <c r="F634" t="s">
-        <v>12152</v>
+        <v>50</v>
       </c>
       <c r="G634" t="s">
-        <v>12152</v>
+        <v>50</v>
       </c>
       <c r="H634" t="s">
-        <v>12152</v>
+        <v>50</v>
       </c>
       <c r="I634" t="s">
-        <v>12152</v>
+        <v>50</v>
       </c>
     </row>
     <row r="635">
       <c r="B635" t="s">
-        <v>12153</v>
+        <v>12154</v>
       </c>
       <c r="C635" t="s">
         <v>78</v>
       </c>
       <c r="D635" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E635" t="s">
         <v>45</v>
       </c>
       <c r="F635" t="s">
-        <v>50</v>
+        <v>11780</v>
       </c>
       <c r="G635" t="s">
-        <v>50</v>
+        <v>11780</v>
       </c>
       <c r="H635" t="s">
-        <v>50</v>
+        <v>11780</v>
       </c>
       <c r="I635" t="s">
-        <v>50</v>
+        <v>11780</v>
       </c>
     </row>
     <row r="636">
       <c r="B636" t="s">
-        <v>12154</v>
+        <v>12208</v>
       </c>
       <c r="C636" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D636" t="s">
         <v>44</v>
@@ -60367,24 +60370,24 @@
         <v>45</v>
       </c>
       <c r="F636" t="s">
-        <v>11780</v>
+        <v>390</v>
       </c>
       <c r="G636" t="s">
-        <v>11780</v>
+        <v>390</v>
       </c>
       <c r="H636" t="s">
-        <v>11780</v>
+        <v>390</v>
       </c>
       <c r="I636" t="s">
-        <v>11780</v>
+        <v>390</v>
       </c>
     </row>
     <row r="637">
       <c r="B637" t="s">
-        <v>12208</v>
+        <v>12209</v>
       </c>
       <c r="C637" t="s">
-        <v>38</v>
+        <v>11926</v>
       </c>
       <c r="D637" t="s">
         <v>44</v>
@@ -60393,50 +60396,50 @@
         <v>45</v>
       </c>
       <c r="F637" t="s">
-        <v>390</v>
+        <v>11930</v>
       </c>
       <c r="G637" t="s">
-        <v>390</v>
+        <v>11930</v>
       </c>
       <c r="H637" t="s">
-        <v>390</v>
+        <v>11930</v>
       </c>
       <c r="I637" t="s">
-        <v>390</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="638">
       <c r="B638" t="s">
-        <v>12209</v>
+        <v>12210</v>
       </c>
       <c r="C638" t="s">
-        <v>11926</v>
+        <v>38</v>
       </c>
       <c r="D638" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E638" t="s">
         <v>45</v>
       </c>
       <c r="F638" t="s">
-        <v>11930</v>
+        <v>11459</v>
       </c>
       <c r="G638" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
       <c r="H638" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
       <c r="I638" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
     </row>
     <row r="639">
       <c r="B639" t="s">
-        <v>12210</v>
+        <v>12226</v>
       </c>
       <c r="C639" t="s">
-        <v>38</v>
+        <v>11926</v>
       </c>
       <c r="D639" t="s">
         <v>49</v>
@@ -60445,76 +60448,76 @@
         <v>45</v>
       </c>
       <c r="F639" t="s">
-        <v>11459</v>
+        <v>50</v>
       </c>
       <c r="G639" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H639" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I639" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="640">
       <c r="B640" t="s">
-        <v>12226</v>
+        <v>12227</v>
       </c>
       <c r="C640" t="s">
         <v>11926</v>
       </c>
       <c r="D640" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E640" t="s">
         <v>45</v>
       </c>
       <c r="F640" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G640" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H640" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I640" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="641">
       <c r="B641" t="s">
-        <v>12227</v>
+        <v>12228</v>
       </c>
       <c r="C641" t="s">
-        <v>11926</v>
+        <v>38</v>
       </c>
       <c r="D641" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E641" t="s">
         <v>45</v>
       </c>
       <c r="F641" t="s">
-        <v>11930</v>
+        <v>11459</v>
       </c>
       <c r="G641" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
       <c r="H641" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
       <c r="I641" t="s">
-        <v>11930</v>
+        <v>47</v>
       </c>
     </row>
     <row r="642">
       <c r="B642" t="s">
-        <v>12228</v>
+        <v>12229</v>
       </c>
       <c r="C642" t="s">
-        <v>38</v>
+        <v>11926</v>
       </c>
       <c r="D642" t="s">
         <v>49</v>
@@ -60523,73 +60526,73 @@
         <v>45</v>
       </c>
       <c r="F642" t="s">
-        <v>11459</v>
+        <v>50</v>
       </c>
       <c r="G642" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H642" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I642" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="643">
       <c r="B643" t="s">
-        <v>12229</v>
+        <v>12230</v>
       </c>
       <c r="C643" t="s">
         <v>11926</v>
       </c>
       <c r="D643" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E643" t="s">
         <v>45</v>
       </c>
       <c r="F643" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G643" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H643" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I643" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="644">
       <c r="B644" t="s">
-        <v>12230</v>
+        <v>12231</v>
       </c>
       <c r="C644" t="s">
-        <v>11926</v>
+        <v>77</v>
       </c>
       <c r="D644" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E644" t="s">
         <v>45</v>
       </c>
       <c r="F644" t="s">
-        <v>11930</v>
+        <v>2574</v>
       </c>
       <c r="G644" t="s">
-        <v>11930</v>
+        <v>2574</v>
       </c>
       <c r="H644" t="s">
-        <v>11930</v>
+        <v>2574</v>
       </c>
       <c r="I644" t="s">
-        <v>11930</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="645">
       <c r="B645" t="s">
-        <v>12231</v>
+        <v>12232</v>
       </c>
       <c r="C645" t="s">
         <v>77</v>
@@ -60601,21 +60604,21 @@
         <v>45</v>
       </c>
       <c r="F645" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="G645" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="H645" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="I645" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="646">
       <c r="B646" t="s">
-        <v>12232</v>
+        <v>12233</v>
       </c>
       <c r="C646" t="s">
         <v>77</v>
@@ -60627,24 +60630,24 @@
         <v>45</v>
       </c>
       <c r="F646" t="s">
-        <v>2570</v>
+        <v>12117</v>
       </c>
       <c r="G646" t="s">
-        <v>2570</v>
+        <v>12117</v>
       </c>
       <c r="H646" t="s">
-        <v>2570</v>
+        <v>12117</v>
       </c>
       <c r="I646" t="s">
-        <v>2570</v>
+        <v>12117</v>
       </c>
     </row>
     <row r="647">
       <c r="B647" t="s">
-        <v>12233</v>
+        <v>12234</v>
       </c>
       <c r="C647" t="s">
-        <v>77</v>
+        <v>11926</v>
       </c>
       <c r="D647" t="s">
         <v>49</v>
@@ -60653,206 +60656,206 @@
         <v>45</v>
       </c>
       <c r="F647" t="s">
-        <v>12117</v>
+        <v>50</v>
       </c>
       <c r="G647" t="s">
-        <v>12117</v>
+        <v>50</v>
       </c>
       <c r="H647" t="s">
-        <v>12117</v>
+        <v>50</v>
       </c>
       <c r="I647" t="s">
-        <v>12117</v>
+        <v>50</v>
       </c>
     </row>
     <row r="648">
       <c r="B648" t="s">
-        <v>12234</v>
+        <v>12235</v>
       </c>
       <c r="C648" t="s">
         <v>11926</v>
       </c>
       <c r="D648" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E648" t="s">
         <v>45</v>
       </c>
       <c r="F648" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G648" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H648" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I648" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="649">
       <c r="B649" t="s">
-        <v>12235</v>
+        <v>12236</v>
       </c>
       <c r="C649" t="s">
         <v>11926</v>
       </c>
       <c r="D649" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E649" t="s">
         <v>45</v>
       </c>
       <c r="F649" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="G649" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="H649" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="I649" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
     </row>
     <row r="650">
       <c r="B650" t="s">
-        <v>12236</v>
+        <v>12237</v>
       </c>
       <c r="C650" t="s">
         <v>11926</v>
       </c>
       <c r="D650" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E650" t="s">
         <v>45</v>
       </c>
       <c r="F650" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G650" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H650" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I650" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="651">
       <c r="B651" t="s">
-        <v>12237</v>
+        <v>12238</v>
       </c>
       <c r="C651" t="s">
         <v>11926</v>
       </c>
       <c r="D651" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E651" t="s">
         <v>45</v>
       </c>
       <c r="F651" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="G651" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="H651" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="I651" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
     </row>
     <row r="652">
       <c r="B652" t="s">
-        <v>12238</v>
+        <v>12239</v>
       </c>
       <c r="C652" t="s">
         <v>11926</v>
       </c>
       <c r="D652" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E652" t="s">
         <v>45</v>
       </c>
       <c r="F652" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G652" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H652" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I652" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="653">
       <c r="B653" t="s">
-        <v>12239</v>
+        <v>12240</v>
       </c>
       <c r="C653" t="s">
         <v>11926</v>
       </c>
       <c r="D653" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E653" t="s">
         <v>45</v>
       </c>
       <c r="F653" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="G653" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="H653" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="I653" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
     </row>
     <row r="654">
       <c r="B654" t="s">
-        <v>12240</v>
+        <v>12241</v>
       </c>
       <c r="C654" t="s">
         <v>11926</v>
       </c>
       <c r="D654" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E654" t="s">
         <v>45</v>
       </c>
       <c r="F654" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="G654" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="H654" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
       <c r="I654" t="s">
-        <v>50</v>
+        <v>11930</v>
       </c>
     </row>
     <row r="655">
       <c r="B655" t="s">
-        <v>12241</v>
+        <v>12250</v>
       </c>
       <c r="C655" t="s">
-        <v>11926</v>
+        <v>78</v>
       </c>
       <c r="D655" t="s">
         <v>44</v>
@@ -60861,47 +60864,47 @@
         <v>45</v>
       </c>
       <c r="F655" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="G655" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="H655" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
       <c r="I655" t="s">
-        <v>11930</v>
+        <v>50</v>
       </c>
     </row>
     <row r="656">
       <c r="B656" t="s">
-        <v>12250</v>
+        <v>12251</v>
       </c>
       <c r="C656" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D656" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E656" t="s">
         <v>45</v>
       </c>
       <c r="F656" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="G656" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="H656" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="I656" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
     </row>
     <row r="657">
       <c r="B657" t="s">
-        <v>12251</v>
+        <v>12252</v>
       </c>
       <c r="C657" t="s">
         <v>38</v>
@@ -60927,7 +60930,7 @@
     </row>
     <row r="658">
       <c r="B658" t="s">
-        <v>12252</v>
+        <v>12253</v>
       </c>
       <c r="C658" t="s">
         <v>38</v>
@@ -60953,7 +60956,7 @@
     </row>
     <row r="659">
       <c r="B659" t="s">
-        <v>12253</v>
+        <v>12254</v>
       </c>
       <c r="C659" t="s">
         <v>38</v>
@@ -60979,7 +60982,7 @@
     </row>
     <row r="660">
       <c r="B660" t="s">
-        <v>12254</v>
+        <v>12255</v>
       </c>
       <c r="C660" t="s">
         <v>38</v>
@@ -61005,7 +61008,7 @@
     </row>
     <row r="661">
       <c r="B661" t="s">
-        <v>12255</v>
+        <v>12256</v>
       </c>
       <c r="C661" t="s">
         <v>38</v>
@@ -61031,7 +61034,7 @@
     </row>
     <row r="662">
       <c r="B662" t="s">
-        <v>12256</v>
+        <v>12257</v>
       </c>
       <c r="C662" t="s">
         <v>38</v>
@@ -61057,7 +61060,7 @@
     </row>
     <row r="663">
       <c r="B663" t="s">
-        <v>12257</v>
+        <v>12258</v>
       </c>
       <c r="C663" t="s">
         <v>38</v>
@@ -61083,7 +61086,7 @@
     </row>
     <row r="664">
       <c r="B664" t="s">
-        <v>12258</v>
+        <v>12259</v>
       </c>
       <c r="C664" t="s">
         <v>38</v>
@@ -61109,7 +61112,7 @@
     </row>
     <row r="665">
       <c r="B665" t="s">
-        <v>12259</v>
+        <v>12260</v>
       </c>
       <c r="C665" t="s">
         <v>38</v>
@@ -61135,13 +61138,13 @@
     </row>
     <row r="666">
       <c r="B666" t="s">
-        <v>12260</v>
+        <v>12261</v>
       </c>
       <c r="C666" t="s">
         <v>38</v>
       </c>
       <c r="D666" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E666" t="s">
         <v>45</v>
@@ -61161,7 +61164,7 @@
     </row>
     <row r="667">
       <c r="B667" t="s">
-        <v>12261</v>
+        <v>12262</v>
       </c>
       <c r="C667" t="s">
         <v>38</v>
@@ -61187,7 +61190,7 @@
     </row>
     <row r="668">
       <c r="B668" t="s">
-        <v>12262</v>
+        <v>12263</v>
       </c>
       <c r="C668" t="s">
         <v>38</v>
@@ -61213,7 +61216,7 @@
     </row>
     <row r="669">
       <c r="B669" t="s">
-        <v>12263</v>
+        <v>12264</v>
       </c>
       <c r="C669" t="s">
         <v>38</v>
@@ -61239,7 +61242,7 @@
     </row>
     <row r="670">
       <c r="B670" t="s">
-        <v>12264</v>
+        <v>12265</v>
       </c>
       <c r="C670" t="s">
         <v>38</v>
@@ -61265,7 +61268,7 @@
     </row>
     <row r="671">
       <c r="B671" t="s">
-        <v>12265</v>
+        <v>12266</v>
       </c>
       <c r="C671" t="s">
         <v>38</v>
@@ -61291,7 +61294,7 @@
     </row>
     <row r="672">
       <c r="B672" t="s">
-        <v>12266</v>
+        <v>12267</v>
       </c>
       <c r="C672" t="s">
         <v>38</v>
@@ -61317,7 +61320,7 @@
     </row>
     <row r="673">
       <c r="B673" t="s">
-        <v>12267</v>
+        <v>12268</v>
       </c>
       <c r="C673" t="s">
         <v>38</v>
@@ -61343,7 +61346,7 @@
     </row>
     <row r="674">
       <c r="B674" t="s">
-        <v>12268</v>
+        <v>12269</v>
       </c>
       <c r="C674" t="s">
         <v>38</v>
@@ -61369,7 +61372,7 @@
     </row>
     <row r="675">
       <c r="B675" t="s">
-        <v>12269</v>
+        <v>12270</v>
       </c>
       <c r="C675" t="s">
         <v>38</v>
@@ -61395,7 +61398,7 @@
     </row>
     <row r="676">
       <c r="B676" t="s">
-        <v>12270</v>
+        <v>12271</v>
       </c>
       <c r="C676" t="s">
         <v>38</v>
@@ -61421,7 +61424,7 @@
     </row>
     <row r="677">
       <c r="B677" t="s">
-        <v>12271</v>
+        <v>12272</v>
       </c>
       <c r="C677" t="s">
         <v>38</v>
@@ -61447,7 +61450,7 @@
     </row>
     <row r="678">
       <c r="B678" t="s">
-        <v>12272</v>
+        <v>12273</v>
       </c>
       <c r="C678" t="s">
         <v>38</v>
@@ -61473,7 +61476,7 @@
     </row>
     <row r="679">
       <c r="B679" t="s">
-        <v>12273</v>
+        <v>12274</v>
       </c>
       <c r="C679" t="s">
         <v>38</v>
@@ -61499,7 +61502,7 @@
     </row>
     <row r="680">
       <c r="B680" t="s">
-        <v>12274</v>
+        <v>12275</v>
       </c>
       <c r="C680" t="s">
         <v>38</v>
@@ -61525,7 +61528,7 @@
     </row>
     <row r="681">
       <c r="B681" t="s">
-        <v>12275</v>
+        <v>12276</v>
       </c>
       <c r="C681" t="s">
         <v>38</v>
@@ -61551,7 +61554,7 @@
     </row>
     <row r="682">
       <c r="B682" t="s">
-        <v>12276</v>
+        <v>12277</v>
       </c>
       <c r="C682" t="s">
         <v>38</v>
@@ -61577,7 +61580,7 @@
     </row>
     <row r="683">
       <c r="B683" t="s">
-        <v>12277</v>
+        <v>12278</v>
       </c>
       <c r="C683" t="s">
         <v>38</v>
@@ -61603,7 +61606,7 @@
     </row>
     <row r="684">
       <c r="B684" t="s">
-        <v>12278</v>
+        <v>12279</v>
       </c>
       <c r="C684" t="s">
         <v>38</v>
@@ -61629,33 +61632,33 @@
     </row>
     <row r="685">
       <c r="B685" t="s">
-        <v>12279</v>
+        <v>12280</v>
       </c>
       <c r="C685" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D685" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E685" t="s">
         <v>45</v>
       </c>
       <c r="F685" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="G685" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="H685" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="I685" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="686">
       <c r="B686" t="s">
-        <v>12280</v>
+        <v>12281</v>
       </c>
       <c r="C686" t="s">
         <v>41</v>
@@ -61667,21 +61670,21 @@
         <v>45</v>
       </c>
       <c r="F686" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G686" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H686" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I686" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="687">
       <c r="B687" t="s">
-        <v>12281</v>
+        <v>12283</v>
       </c>
       <c r="C687" t="s">
         <v>41</v>
@@ -61693,50 +61696,50 @@
         <v>45</v>
       </c>
       <c r="F687" t="s">
-        <v>238</v>
+        <v>12284</v>
       </c>
       <c r="G687" t="s">
-        <v>238</v>
+        <v>12284</v>
       </c>
       <c r="H687" t="s">
-        <v>238</v>
+        <v>12284</v>
       </c>
       <c r="I687" t="s">
-        <v>238</v>
+        <v>12284</v>
       </c>
     </row>
     <row r="688">
       <c r="B688" t="s">
-        <v>12283</v>
+        <v>12286</v>
       </c>
       <c r="C688" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D688" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E688" t="s">
         <v>45</v>
       </c>
       <c r="F688" t="s">
-        <v>12284</v>
+        <v>1294</v>
       </c>
       <c r="G688" t="s">
-        <v>12284</v>
+        <v>12048</v>
       </c>
       <c r="H688" t="s">
-        <v>12284</v>
+        <v>12048</v>
       </c>
       <c r="I688" t="s">
-        <v>12284</v>
+        <v>12048</v>
       </c>
     </row>
     <row r="689">
       <c r="B689" t="s">
-        <v>12285</v>
+        <v>12291</v>
       </c>
       <c r="C689" t="s">
-        <v>1594</v>
+        <v>38</v>
       </c>
       <c r="D689" t="s">
         <v>44</v>
@@ -61745,24 +61748,24 @@
         <v>45</v>
       </c>
       <c r="F689" t="s">
-        <v>1294</v>
+        <v>50</v>
       </c>
       <c r="G689" t="s">
-        <v>1294</v>
+        <v>50</v>
       </c>
       <c r="H689" t="s">
-        <v>1294</v>
+        <v>50</v>
       </c>
       <c r="I689" t="s">
-        <v>1294</v>
+        <v>50</v>
       </c>
     </row>
     <row r="690">
       <c r="B690" t="s">
-        <v>12286</v>
+        <v>12293</v>
       </c>
       <c r="C690" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D690" t="s">
         <v>44</v>
@@ -61771,47 +61774,47 @@
         <v>45</v>
       </c>
       <c r="F690" t="s">
-        <v>1294</v>
+        <v>390</v>
       </c>
       <c r="G690" t="s">
-        <v>12048</v>
+        <v>284</v>
       </c>
       <c r="H690" t="s">
-        <v>12048</v>
+        <v>284</v>
       </c>
       <c r="I690" t="s">
-        <v>12048</v>
+        <v>284</v>
       </c>
     </row>
     <row r="691">
       <c r="B691" t="s">
-        <v>12289</v>
+        <v>12299</v>
       </c>
       <c r="C691" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D691" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E691" t="s">
         <v>45</v>
       </c>
       <c r="F691" t="s">
-        <v>12294</v>
+        <v>50</v>
       </c>
       <c r="G691" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="H691" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="I691" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="692">
       <c r="B692" t="s">
-        <v>12291</v>
+        <v>12300</v>
       </c>
       <c r="C692" t="s">
         <v>38</v>
@@ -61823,21 +61826,21 @@
         <v>45</v>
       </c>
       <c r="F692" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G692" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H692" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I692" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="693">
       <c r="B693" t="s">
-        <v>12293</v>
+        <v>12303</v>
       </c>
       <c r="C693" t="s">
         <v>38</v>
@@ -61849,21 +61852,21 @@
         <v>45</v>
       </c>
       <c r="F693" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G693" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H693" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I693" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="694">
       <c r="B694" t="s">
-        <v>12299</v>
+        <v>12304</v>
       </c>
       <c r="C694" t="s">
         <v>38</v>
@@ -61875,21 +61878,21 @@
         <v>45</v>
       </c>
       <c r="F694" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G694" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H694" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I694" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="695">
       <c r="B695" t="s">
-        <v>12300</v>
+        <v>12305</v>
       </c>
       <c r="C695" t="s">
         <v>38</v>
@@ -61901,21 +61904,21 @@
         <v>45</v>
       </c>
       <c r="F695" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G695" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H695" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I695" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="696">
       <c r="B696" t="s">
-        <v>12303</v>
+        <v>12306</v>
       </c>
       <c r="C696" t="s">
         <v>38</v>
@@ -61927,21 +61930,21 @@
         <v>45</v>
       </c>
       <c r="F696" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G696" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H696" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I696" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="697">
       <c r="B697" t="s">
-        <v>12304</v>
+        <v>12307</v>
       </c>
       <c r="C697" t="s">
         <v>38</v>
@@ -61953,21 +61956,21 @@
         <v>45</v>
       </c>
       <c r="F697" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G697" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H697" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I697" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="698">
       <c r="B698" t="s">
-        <v>12305</v>
+        <v>12308</v>
       </c>
       <c r="C698" t="s">
         <v>38</v>
@@ -61979,21 +61982,21 @@
         <v>45</v>
       </c>
       <c r="F698" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G698" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H698" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I698" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="699">
       <c r="B699" t="s">
-        <v>12306</v>
+        <v>12309</v>
       </c>
       <c r="C699" t="s">
         <v>38</v>
@@ -62005,21 +62008,21 @@
         <v>45</v>
       </c>
       <c r="F699" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G699" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H699" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I699" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="700">
       <c r="B700" t="s">
-        <v>12307</v>
+        <v>12310</v>
       </c>
       <c r="C700" t="s">
         <v>38</v>
@@ -62031,21 +62034,21 @@
         <v>45</v>
       </c>
       <c r="F700" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G700" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H700" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I700" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="701">
       <c r="B701" t="s">
-        <v>12308</v>
+        <v>12311</v>
       </c>
       <c r="C701" t="s">
         <v>38</v>
@@ -62057,21 +62060,21 @@
         <v>45</v>
       </c>
       <c r="F701" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G701" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H701" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I701" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="702">
       <c r="B702" t="s">
-        <v>12309</v>
+        <v>12312</v>
       </c>
       <c r="C702" t="s">
         <v>38</v>
@@ -62083,21 +62086,21 @@
         <v>45</v>
       </c>
       <c r="F702" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G702" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H702" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I702" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="703">
       <c r="B703" t="s">
-        <v>12310</v>
+        <v>12313</v>
       </c>
       <c r="C703" t="s">
         <v>38</v>
@@ -62109,21 +62112,21 @@
         <v>45</v>
       </c>
       <c r="F703" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G703" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H703" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I703" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="704">
       <c r="B704" t="s">
-        <v>12311</v>
+        <v>12314</v>
       </c>
       <c r="C704" t="s">
         <v>38</v>
@@ -62135,21 +62138,21 @@
         <v>45</v>
       </c>
       <c r="F704" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G704" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H704" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I704" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="705">
       <c r="B705" t="s">
-        <v>12312</v>
+        <v>12315</v>
       </c>
       <c r="C705" t="s">
         <v>38</v>
@@ -62161,21 +62164,21 @@
         <v>45</v>
       </c>
       <c r="F705" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G705" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H705" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I705" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="706">
       <c r="B706" t="s">
-        <v>12313</v>
+        <v>12316</v>
       </c>
       <c r="C706" t="s">
         <v>38</v>
@@ -62187,21 +62190,21 @@
         <v>45</v>
       </c>
       <c r="F706" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G706" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H706" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I706" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="707">
       <c r="B707" t="s">
-        <v>12314</v>
+        <v>12317</v>
       </c>
       <c r="C707" t="s">
         <v>38</v>
@@ -62213,21 +62216,21 @@
         <v>45</v>
       </c>
       <c r="F707" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G707" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H707" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I707" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="708">
       <c r="B708" t="s">
-        <v>12315</v>
+        <v>12318</v>
       </c>
       <c r="C708" t="s">
         <v>38</v>
@@ -62239,21 +62242,21 @@
         <v>45</v>
       </c>
       <c r="F708" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G708" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H708" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I708" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="709">
       <c r="B709" t="s">
-        <v>12316</v>
+        <v>12319</v>
       </c>
       <c r="C709" t="s">
         <v>38</v>
@@ -62265,21 +62268,21 @@
         <v>45</v>
       </c>
       <c r="F709" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G709" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H709" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I709" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="710">
       <c r="B710" t="s">
-        <v>12317</v>
+        <v>12320</v>
       </c>
       <c r="C710" t="s">
         <v>38</v>
@@ -62291,21 +62294,21 @@
         <v>45</v>
       </c>
       <c r="F710" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G710" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H710" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I710" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="711">
       <c r="B711" t="s">
-        <v>12318</v>
+        <v>12321</v>
       </c>
       <c r="C711" t="s">
         <v>38</v>
@@ -62317,21 +62320,21 @@
         <v>45</v>
       </c>
       <c r="F711" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G711" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H711" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I711" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="712">
       <c r="B712" t="s">
-        <v>12319</v>
+        <v>12322</v>
       </c>
       <c r="C712" t="s">
         <v>38</v>
@@ -62343,21 +62346,21 @@
         <v>45</v>
       </c>
       <c r="F712" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G712" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H712" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I712" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="713">
       <c r="B713" t="s">
-        <v>12320</v>
+        <v>12323</v>
       </c>
       <c r="C713" t="s">
         <v>38</v>
@@ -62369,21 +62372,21 @@
         <v>45</v>
       </c>
       <c r="F713" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G713" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H713" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I713" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="714">
       <c r="B714" t="s">
-        <v>12321</v>
+        <v>12324</v>
       </c>
       <c r="C714" t="s">
         <v>38</v>
@@ -62395,21 +62398,21 @@
         <v>45</v>
       </c>
       <c r="F714" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G714" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H714" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I714" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="715">
       <c r="B715" t="s">
-        <v>12322</v>
+        <v>12325</v>
       </c>
       <c r="C715" t="s">
         <v>38</v>
@@ -62421,21 +62424,21 @@
         <v>45</v>
       </c>
       <c r="F715" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G715" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H715" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I715" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="716">
       <c r="B716" t="s">
-        <v>12323</v>
+        <v>12326</v>
       </c>
       <c r="C716" t="s">
         <v>38</v>
@@ -62447,21 +62450,21 @@
         <v>45</v>
       </c>
       <c r="F716" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G716" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H716" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I716" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="717">
       <c r="B717" t="s">
-        <v>12324</v>
+        <v>12327</v>
       </c>
       <c r="C717" t="s">
         <v>38</v>
@@ -62473,21 +62476,21 @@
         <v>45</v>
       </c>
       <c r="F717" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G717" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H717" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I717" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="718">
       <c r="B718" t="s">
-        <v>12325</v>
+        <v>12328</v>
       </c>
       <c r="C718" t="s">
         <v>38</v>
@@ -62499,21 +62502,21 @@
         <v>45</v>
       </c>
       <c r="F718" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G718" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H718" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I718" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="719">
       <c r="B719" t="s">
-        <v>12326</v>
+        <v>12329</v>
       </c>
       <c r="C719" t="s">
         <v>38</v>
@@ -62525,21 +62528,21 @@
         <v>45</v>
       </c>
       <c r="F719" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G719" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H719" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I719" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="720">
       <c r="B720" t="s">
-        <v>12327</v>
+        <v>12330</v>
       </c>
       <c r="C720" t="s">
         <v>38</v>
@@ -62551,21 +62554,21 @@
         <v>45</v>
       </c>
       <c r="F720" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G720" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H720" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I720" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="721">
       <c r="B721" t="s">
-        <v>12328</v>
+        <v>12331</v>
       </c>
       <c r="C721" t="s">
         <v>38</v>
@@ -62577,21 +62580,21 @@
         <v>45</v>
       </c>
       <c r="F721" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G721" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H721" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I721" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="722">
       <c r="B722" t="s">
-        <v>12329</v>
+        <v>12332</v>
       </c>
       <c r="C722" t="s">
         <v>38</v>
@@ -62603,21 +62606,21 @@
         <v>45</v>
       </c>
       <c r="F722" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G722" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H722" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I722" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="723">
       <c r="B723" t="s">
-        <v>12330</v>
+        <v>12333</v>
       </c>
       <c r="C723" t="s">
         <v>38</v>
@@ -62629,21 +62632,21 @@
         <v>45</v>
       </c>
       <c r="F723" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G723" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H723" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I723" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="724">
       <c r="B724" t="s">
-        <v>12331</v>
+        <v>12334</v>
       </c>
       <c r="C724" t="s">
         <v>38</v>
@@ -62655,21 +62658,21 @@
         <v>45</v>
       </c>
       <c r="F724" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G724" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H724" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I724" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="725">
       <c r="B725" t="s">
-        <v>12332</v>
+        <v>12335</v>
       </c>
       <c r="C725" t="s">
         <v>38</v>
@@ -62681,21 +62684,21 @@
         <v>45</v>
       </c>
       <c r="F725" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G725" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H725" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I725" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="726">
       <c r="B726" t="s">
-        <v>12333</v>
+        <v>12336</v>
       </c>
       <c r="C726" t="s">
         <v>38</v>
@@ -62707,21 +62710,21 @@
         <v>45</v>
       </c>
       <c r="F726" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G726" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H726" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I726" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="727">
       <c r="B727" t="s">
-        <v>12334</v>
+        <v>12337</v>
       </c>
       <c r="C727" t="s">
         <v>38</v>
@@ -62733,21 +62736,21 @@
         <v>45</v>
       </c>
       <c r="F727" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G727" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H727" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I727" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="728">
       <c r="B728" t="s">
-        <v>12335</v>
+        <v>12338</v>
       </c>
       <c r="C728" t="s">
         <v>38</v>
@@ -62759,21 +62762,21 @@
         <v>45</v>
       </c>
       <c r="F728" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G728" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H728" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I728" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="729">
       <c r="B729" t="s">
-        <v>12336</v>
+        <v>12339</v>
       </c>
       <c r="C729" t="s">
         <v>38</v>
@@ -62785,21 +62788,21 @@
         <v>45</v>
       </c>
       <c r="F729" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G729" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H729" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I729" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="730">
       <c r="B730" t="s">
-        <v>12337</v>
+        <v>12340</v>
       </c>
       <c r="C730" t="s">
         <v>38</v>
@@ -62811,21 +62814,21 @@
         <v>45</v>
       </c>
       <c r="F730" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G730" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H730" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I730" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="731">
       <c r="B731" t="s">
-        <v>12338</v>
+        <v>12341</v>
       </c>
       <c r="C731" t="s">
         <v>38</v>
@@ -62837,21 +62840,21 @@
         <v>45</v>
       </c>
       <c r="F731" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G731" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H731" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I731" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="732">
       <c r="B732" t="s">
-        <v>12339</v>
+        <v>12342</v>
       </c>
       <c r="C732" t="s">
         <v>38</v>
@@ -62863,21 +62866,21 @@
         <v>45</v>
       </c>
       <c r="F732" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G732" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H732" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I732" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="733">
       <c r="B733" t="s">
-        <v>12340</v>
+        <v>12343</v>
       </c>
       <c r="C733" t="s">
         <v>38</v>
@@ -62889,21 +62892,21 @@
         <v>45</v>
       </c>
       <c r="F733" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G733" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H733" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I733" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="734">
       <c r="B734" t="s">
-        <v>12341</v>
+        <v>12344</v>
       </c>
       <c r="C734" t="s">
         <v>38</v>
@@ -62915,21 +62918,21 @@
         <v>45</v>
       </c>
       <c r="F734" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G734" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H734" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I734" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="735">
       <c r="B735" t="s">
-        <v>12342</v>
+        <v>12345</v>
       </c>
       <c r="C735" t="s">
         <v>38</v>
@@ -62941,21 +62944,21 @@
         <v>45</v>
       </c>
       <c r="F735" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G735" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H735" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I735" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="736">
       <c r="B736" t="s">
-        <v>12343</v>
+        <v>12346</v>
       </c>
       <c r="C736" t="s">
         <v>38</v>
@@ -62967,21 +62970,21 @@
         <v>45</v>
       </c>
       <c r="F736" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G736" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H736" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I736" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="737">
       <c r="B737" t="s">
-        <v>12344</v>
+        <v>12347</v>
       </c>
       <c r="C737" t="s">
         <v>38</v>
@@ -62993,21 +62996,21 @@
         <v>45</v>
       </c>
       <c r="F737" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G737" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H737" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I737" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="738">
       <c r="B738" t="s">
-        <v>12345</v>
+        <v>12348</v>
       </c>
       <c r="C738" t="s">
         <v>38</v>
@@ -63019,21 +63022,21 @@
         <v>45</v>
       </c>
       <c r="F738" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G738" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H738" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I738" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="739">
       <c r="B739" t="s">
-        <v>12346</v>
+        <v>12349</v>
       </c>
       <c r="C739" t="s">
         <v>38</v>
@@ -63045,21 +63048,21 @@
         <v>45</v>
       </c>
       <c r="F739" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G739" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H739" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I739" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="740">
       <c r="B740" t="s">
-        <v>12347</v>
+        <v>12350</v>
       </c>
       <c r="C740" t="s">
         <v>38</v>
@@ -63071,21 +63074,21 @@
         <v>45</v>
       </c>
       <c r="F740" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G740" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H740" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I740" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="741">
       <c r="B741" t="s">
-        <v>12348</v>
+        <v>12351</v>
       </c>
       <c r="C741" t="s">
         <v>38</v>
@@ -63097,21 +63100,21 @@
         <v>45</v>
       </c>
       <c r="F741" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G741" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H741" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I741" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="742">
       <c r="B742" t="s">
-        <v>12349</v>
+        <v>12352</v>
       </c>
       <c r="C742" t="s">
         <v>38</v>
@@ -63123,21 +63126,21 @@
         <v>45</v>
       </c>
       <c r="F742" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G742" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H742" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I742" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="743">
       <c r="B743" t="s">
-        <v>12350</v>
+        <v>12353</v>
       </c>
       <c r="C743" t="s">
         <v>38</v>
@@ -63149,21 +63152,21 @@
         <v>45</v>
       </c>
       <c r="F743" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G743" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H743" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I743" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="744">
       <c r="B744" t="s">
-        <v>12351</v>
+        <v>12354</v>
       </c>
       <c r="C744" t="s">
         <v>38</v>
@@ -63175,21 +63178,21 @@
         <v>45</v>
       </c>
       <c r="F744" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G744" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H744" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I744" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="745">
       <c r="B745" t="s">
-        <v>12352</v>
+        <v>12355</v>
       </c>
       <c r="C745" t="s">
         <v>38</v>
@@ -63201,21 +63204,21 @@
         <v>45</v>
       </c>
       <c r="F745" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G745" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H745" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I745" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="746">
       <c r="B746" t="s">
-        <v>12353</v>
+        <v>12356</v>
       </c>
       <c r="C746" t="s">
         <v>38</v>
@@ -63227,21 +63230,21 @@
         <v>45</v>
       </c>
       <c r="F746" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G746" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H746" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I746" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="747">
       <c r="B747" t="s">
-        <v>12354</v>
+        <v>12357</v>
       </c>
       <c r="C747" t="s">
         <v>38</v>
@@ -63253,21 +63256,21 @@
         <v>45</v>
       </c>
       <c r="F747" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G747" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H747" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I747" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="748">
       <c r="B748" t="s">
-        <v>12355</v>
+        <v>12358</v>
       </c>
       <c r="C748" t="s">
         <v>38</v>
@@ -63279,21 +63282,21 @@
         <v>45</v>
       </c>
       <c r="F748" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G748" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H748" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I748" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="749">
       <c r="B749" t="s">
-        <v>12356</v>
+        <v>12359</v>
       </c>
       <c r="C749" t="s">
         <v>38</v>
@@ -63305,21 +63308,21 @@
         <v>45</v>
       </c>
       <c r="F749" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G749" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H749" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I749" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="750">
       <c r="B750" t="s">
-        <v>12357</v>
+        <v>12360</v>
       </c>
       <c r="C750" t="s">
         <v>38</v>
@@ -63331,21 +63334,21 @@
         <v>45</v>
       </c>
       <c r="F750" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G750" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H750" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I750" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="751">
       <c r="B751" t="s">
-        <v>12358</v>
+        <v>12361</v>
       </c>
       <c r="C751" t="s">
         <v>38</v>
@@ -63357,21 +63360,21 @@
         <v>45</v>
       </c>
       <c r="F751" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G751" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H751" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I751" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="752">
       <c r="B752" t="s">
-        <v>12359</v>
+        <v>12362</v>
       </c>
       <c r="C752" t="s">
         <v>38</v>
@@ -63383,21 +63386,21 @@
         <v>45</v>
       </c>
       <c r="F752" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G752" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H752" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I752" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="753">
       <c r="B753" t="s">
-        <v>12360</v>
+        <v>12363</v>
       </c>
       <c r="C753" t="s">
         <v>38</v>
@@ -63409,24 +63412,24 @@
         <v>45</v>
       </c>
       <c r="F753" t="s">
-        <v>390</v>
+        <v>47</v>
       </c>
       <c r="G753" t="s">
-        <v>284</v>
+        <v>47</v>
       </c>
       <c r="H753" t="s">
-        <v>284</v>
+        <v>47</v>
       </c>
       <c r="I753" t="s">
-        <v>284</v>
+        <v>47</v>
       </c>
     </row>
     <row r="754">
       <c r="B754" t="s">
-        <v>12361</v>
+        <v>12285</v>
       </c>
       <c r="C754" t="s">
-        <v>38</v>
+        <v>1594</v>
       </c>
       <c r="D754" t="s">
         <v>44</v>
@@ -63435,45 +63438,70 @@
         <v>45</v>
       </c>
       <c r="F754" t="s">
-        <v>50</v>
+        <v>1294</v>
       </c>
       <c r="G754" t="s">
-        <v>50</v>
+        <v>1294</v>
       </c>
       <c r="H754" t="s">
-        <v>50</v>
+        <v>1294</v>
       </c>
       <c r="I754" t="s">
-        <v>50</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="755">
       <c r="B755" t="s">
-        <v>12362</v>
+        <v>12101</v>
       </c>
       <c r="C755" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D755" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E755" t="s">
         <v>45</v>
       </c>
       <c r="F755" t="s">
-        <v>390</v>
+        <v>12102</v>
       </c>
       <c r="G755" t="s">
-        <v>284</v>
+        <v>12102</v>
       </c>
       <c r="H755" t="s">
-        <v>284</v>
+        <v>12102</v>
       </c>
       <c r="I755" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="756"/>
+        <v>12102</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="B756" t="s">
+        <v>12289</v>
+      </c>
+      <c r="C756" t="s">
+        <v>40</v>
+      </c>
+      <c r="D756" t="s">
+        <v>49</v>
+      </c>
+      <c r="E756" t="s">
+        <v>45</v>
+      </c>
+      <c r="F756" t="s">
+        <v>12294</v>
+      </c>
+      <c r="G756" t="s">
+        <v>12102</v>
+      </c>
+      <c r="H756" t="s">
+        <v>12102</v>
+      </c>
+      <c r="I756" t="s">
+        <v>12102</v>
+      </c>
+    </row>
     <row r="757"/>
     <row r="758"/>
     <row r="759"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-08-14 22-17-32
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439188" uniqueCount="12364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6457780" uniqueCount="12374">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41896,6 +41896,36 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4175</t>
   </si>
 </sst>
 </file>
@@ -63502,16 +63532,266 @@
         <v>12102</v>
       </c>
     </row>
-    <row r="757"/>
-    <row r="758"/>
-    <row r="759"/>
-    <row r="760"/>
-    <row r="761"/>
-    <row r="762"/>
-    <row r="763"/>
-    <row r="764"/>
-    <row r="765"/>
-    <row r="766"/>
+    <row r="757">
+      <c r="B757" t="s">
+        <v>12364</v>
+      </c>
+      <c r="C757" t="s">
+        <v>38</v>
+      </c>
+      <c r="D757" t="s">
+        <v>49</v>
+      </c>
+      <c r="E757" t="s">
+        <v>45</v>
+      </c>
+      <c r="F757" t="s">
+        <v>50</v>
+      </c>
+      <c r="G757" t="s">
+        <v>50</v>
+      </c>
+      <c r="H757" t="s">
+        <v>50</v>
+      </c>
+      <c r="I757" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="B758" t="s">
+        <v>12365</v>
+      </c>
+      <c r="C758" t="s">
+        <v>38</v>
+      </c>
+      <c r="D758" t="s">
+        <v>44</v>
+      </c>
+      <c r="E758" t="s">
+        <v>45</v>
+      </c>
+      <c r="F758" t="s">
+        <v>390</v>
+      </c>
+      <c r="G758" t="s">
+        <v>390</v>
+      </c>
+      <c r="H758" t="s">
+        <v>390</v>
+      </c>
+      <c r="I758" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="B759" t="s">
+        <v>12366</v>
+      </c>
+      <c r="C759" t="s">
+        <v>38</v>
+      </c>
+      <c r="D759" t="s">
+        <v>49</v>
+      </c>
+      <c r="E759" t="s">
+        <v>45</v>
+      </c>
+      <c r="F759" t="s">
+        <v>50</v>
+      </c>
+      <c r="G759" t="s">
+        <v>50</v>
+      </c>
+      <c r="H759" t="s">
+        <v>50</v>
+      </c>
+      <c r="I759" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="B760" t="s">
+        <v>12367</v>
+      </c>
+      <c r="C760" t="s">
+        <v>38</v>
+      </c>
+      <c r="D760" t="s">
+        <v>44</v>
+      </c>
+      <c r="E760" t="s">
+        <v>45</v>
+      </c>
+      <c r="F760" t="s">
+        <v>390</v>
+      </c>
+      <c r="G760" t="s">
+        <v>390</v>
+      </c>
+      <c r="H760" t="s">
+        <v>390</v>
+      </c>
+      <c r="I760" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="B761" t="s">
+        <v>12368</v>
+      </c>
+      <c r="C761" t="s">
+        <v>38</v>
+      </c>
+      <c r="D761" t="s">
+        <v>49</v>
+      </c>
+      <c r="E761" t="s">
+        <v>45</v>
+      </c>
+      <c r="F761" t="s">
+        <v>50</v>
+      </c>
+      <c r="G761" t="s">
+        <v>50</v>
+      </c>
+      <c r="H761" t="s">
+        <v>50</v>
+      </c>
+      <c r="I761" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="B762" t="s">
+        <v>12369</v>
+      </c>
+      <c r="C762" t="s">
+        <v>38</v>
+      </c>
+      <c r="D762" t="s">
+        <v>44</v>
+      </c>
+      <c r="E762" t="s">
+        <v>45</v>
+      </c>
+      <c r="F762" t="s">
+        <v>390</v>
+      </c>
+      <c r="G762" t="s">
+        <v>390</v>
+      </c>
+      <c r="H762" t="s">
+        <v>390</v>
+      </c>
+      <c r="I762" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="B763" t="s">
+        <v>12370</v>
+      </c>
+      <c r="C763" t="s">
+        <v>38</v>
+      </c>
+      <c r="D763" t="s">
+        <v>49</v>
+      </c>
+      <c r="E763" t="s">
+        <v>45</v>
+      </c>
+      <c r="F763" t="s">
+        <v>50</v>
+      </c>
+      <c r="G763" t="s">
+        <v>50</v>
+      </c>
+      <c r="H763" t="s">
+        <v>50</v>
+      </c>
+      <c r="I763" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="B764" t="s">
+        <v>12371</v>
+      </c>
+      <c r="C764" t="s">
+        <v>38</v>
+      </c>
+      <c r="D764" t="s">
+        <v>44</v>
+      </c>
+      <c r="E764" t="s">
+        <v>45</v>
+      </c>
+      <c r="F764" t="s">
+        <v>390</v>
+      </c>
+      <c r="G764" t="s">
+        <v>390</v>
+      </c>
+      <c r="H764" t="s">
+        <v>390</v>
+      </c>
+      <c r="I764" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="B765" t="s">
+        <v>12372</v>
+      </c>
+      <c r="C765" t="s">
+        <v>38</v>
+      </c>
+      <c r="D765" t="s">
+        <v>49</v>
+      </c>
+      <c r="E765" t="s">
+        <v>45</v>
+      </c>
+      <c r="F765" t="s">
+        <v>50</v>
+      </c>
+      <c r="G765" t="s">
+        <v>50</v>
+      </c>
+      <c r="H765" t="s">
+        <v>50</v>
+      </c>
+      <c r="I765" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="B766" t="s">
+        <v>12373</v>
+      </c>
+      <c r="C766" t="s">
+        <v>38</v>
+      </c>
+      <c r="D766" t="s">
+        <v>44</v>
+      </c>
+      <c r="E766" t="s">
+        <v>45</v>
+      </c>
+      <c r="F766" t="s">
+        <v>390</v>
+      </c>
+      <c r="G766" t="s">
+        <v>390</v>
+      </c>
+      <c r="H766" t="s">
+        <v>390</v>
+      </c>
+      <c r="I766" t="s">
+        <v>390</v>
+      </c>
+    </row>
     <row r="767"/>
     <row r="768"/>
     <row r="769"/>

</xml_diff>

<commit_message>
Project Updated at: 2024-08-16 20-00-51
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6457780" uniqueCount="12374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6541504" uniqueCount="12381">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41926,6 +41926,27 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo de receita em ZERO!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4181</t>
   </si>
 </sst>
 </file>
@@ -58840,7 +58861,7 @@
         <v>45</v>
       </c>
       <c r="F576" t="s">
-        <v>12065</v>
+        <v>12376</v>
       </c>
       <c r="G576" t="s">
         <v>12065</v>
@@ -61818,7 +61839,7 @@
     </row>
     <row r="691">
       <c r="B691" t="s">
-        <v>12299</v>
+        <v>12303</v>
       </c>
       <c r="C691" t="s">
         <v>38</v>
@@ -61844,7 +61865,7 @@
     </row>
     <row r="692">
       <c r="B692" t="s">
-        <v>12300</v>
+        <v>12304</v>
       </c>
       <c r="C692" t="s">
         <v>38</v>
@@ -61870,7 +61891,7 @@
     </row>
     <row r="693">
       <c r="B693" t="s">
-        <v>12303</v>
+        <v>12305</v>
       </c>
       <c r="C693" t="s">
         <v>38</v>
@@ -61896,7 +61917,7 @@
     </row>
     <row r="694">
       <c r="B694" t="s">
-        <v>12304</v>
+        <v>12306</v>
       </c>
       <c r="C694" t="s">
         <v>38</v>
@@ -61922,7 +61943,7 @@
     </row>
     <row r="695">
       <c r="B695" t="s">
-        <v>12305</v>
+        <v>12307</v>
       </c>
       <c r="C695" t="s">
         <v>38</v>
@@ -61948,7 +61969,7 @@
     </row>
     <row r="696">
       <c r="B696" t="s">
-        <v>12306</v>
+        <v>12308</v>
       </c>
       <c r="C696" t="s">
         <v>38</v>
@@ -61974,7 +61995,7 @@
     </row>
     <row r="697">
       <c r="B697" t="s">
-        <v>12307</v>
+        <v>12309</v>
       </c>
       <c r="C697" t="s">
         <v>38</v>
@@ -62000,7 +62021,7 @@
     </row>
     <row r="698">
       <c r="B698" t="s">
-        <v>12308</v>
+        <v>12310</v>
       </c>
       <c r="C698" t="s">
         <v>38</v>
@@ -62026,7 +62047,7 @@
     </row>
     <row r="699">
       <c r="B699" t="s">
-        <v>12309</v>
+        <v>12311</v>
       </c>
       <c r="C699" t="s">
         <v>38</v>
@@ -62052,7 +62073,7 @@
     </row>
     <row r="700">
       <c r="B700" t="s">
-        <v>12310</v>
+        <v>12312</v>
       </c>
       <c r="C700" t="s">
         <v>38</v>
@@ -62078,7 +62099,7 @@
     </row>
     <row r="701">
       <c r="B701" t="s">
-        <v>12311</v>
+        <v>12313</v>
       </c>
       <c r="C701" t="s">
         <v>38</v>
@@ -62104,7 +62125,7 @@
     </row>
     <row r="702">
       <c r="B702" t="s">
-        <v>12312</v>
+        <v>12314</v>
       </c>
       <c r="C702" t="s">
         <v>38</v>
@@ -62130,7 +62151,7 @@
     </row>
     <row r="703">
       <c r="B703" t="s">
-        <v>12313</v>
+        <v>12315</v>
       </c>
       <c r="C703" t="s">
         <v>38</v>
@@ -62156,7 +62177,7 @@
     </row>
     <row r="704">
       <c r="B704" t="s">
-        <v>12314</v>
+        <v>12316</v>
       </c>
       <c r="C704" t="s">
         <v>38</v>
@@ -62182,7 +62203,7 @@
     </row>
     <row r="705">
       <c r="B705" t="s">
-        <v>12315</v>
+        <v>12317</v>
       </c>
       <c r="C705" t="s">
         <v>38</v>
@@ -62208,7 +62229,7 @@
     </row>
     <row r="706">
       <c r="B706" t="s">
-        <v>12316</v>
+        <v>12318</v>
       </c>
       <c r="C706" t="s">
         <v>38</v>
@@ -62234,7 +62255,7 @@
     </row>
     <row r="707">
       <c r="B707" t="s">
-        <v>12317</v>
+        <v>12319</v>
       </c>
       <c r="C707" t="s">
         <v>38</v>
@@ -62260,7 +62281,7 @@
     </row>
     <row r="708">
       <c r="B708" t="s">
-        <v>12318</v>
+        <v>12320</v>
       </c>
       <c r="C708" t="s">
         <v>38</v>
@@ -62286,7 +62307,7 @@
     </row>
     <row r="709">
       <c r="B709" t="s">
-        <v>12319</v>
+        <v>12321</v>
       </c>
       <c r="C709" t="s">
         <v>38</v>
@@ -62312,7 +62333,7 @@
     </row>
     <row r="710">
       <c r="B710" t="s">
-        <v>12320</v>
+        <v>12322</v>
       </c>
       <c r="C710" t="s">
         <v>38</v>
@@ -62338,7 +62359,7 @@
     </row>
     <row r="711">
       <c r="B711" t="s">
-        <v>12321</v>
+        <v>12323</v>
       </c>
       <c r="C711" t="s">
         <v>38</v>
@@ -62364,7 +62385,7 @@
     </row>
     <row r="712">
       <c r="B712" t="s">
-        <v>12322</v>
+        <v>12324</v>
       </c>
       <c r="C712" t="s">
         <v>38</v>
@@ -62390,7 +62411,7 @@
     </row>
     <row r="713">
       <c r="B713" t="s">
-        <v>12323</v>
+        <v>12325</v>
       </c>
       <c r="C713" t="s">
         <v>38</v>
@@ -62416,7 +62437,7 @@
     </row>
     <row r="714">
       <c r="B714" t="s">
-        <v>12324</v>
+        <v>12326</v>
       </c>
       <c r="C714" t="s">
         <v>38</v>
@@ -62442,7 +62463,7 @@
     </row>
     <row r="715">
       <c r="B715" t="s">
-        <v>12325</v>
+        <v>12327</v>
       </c>
       <c r="C715" t="s">
         <v>38</v>
@@ -62468,7 +62489,7 @@
     </row>
     <row r="716">
       <c r="B716" t="s">
-        <v>12326</v>
+        <v>12328</v>
       </c>
       <c r="C716" t="s">
         <v>38</v>
@@ -62494,7 +62515,7 @@
     </row>
     <row r="717">
       <c r="B717" t="s">
-        <v>12327</v>
+        <v>12329</v>
       </c>
       <c r="C717" t="s">
         <v>38</v>
@@ -62520,7 +62541,7 @@
     </row>
     <row r="718">
       <c r="B718" t="s">
-        <v>12328</v>
+        <v>12330</v>
       </c>
       <c r="C718" t="s">
         <v>38</v>
@@ -62546,7 +62567,7 @@
     </row>
     <row r="719">
       <c r="B719" t="s">
-        <v>12329</v>
+        <v>12331</v>
       </c>
       <c r="C719" t="s">
         <v>38</v>
@@ -62572,7 +62593,7 @@
     </row>
     <row r="720">
       <c r="B720" t="s">
-        <v>12330</v>
+        <v>12332</v>
       </c>
       <c r="C720" t="s">
         <v>38</v>
@@ -62598,7 +62619,7 @@
     </row>
     <row r="721">
       <c r="B721" t="s">
-        <v>12331</v>
+        <v>12333</v>
       </c>
       <c r="C721" t="s">
         <v>38</v>
@@ -62624,7 +62645,7 @@
     </row>
     <row r="722">
       <c r="B722" t="s">
-        <v>12332</v>
+        <v>12334</v>
       </c>
       <c r="C722" t="s">
         <v>38</v>
@@ -62650,7 +62671,7 @@
     </row>
     <row r="723">
       <c r="B723" t="s">
-        <v>12333</v>
+        <v>12335</v>
       </c>
       <c r="C723" t="s">
         <v>38</v>
@@ -62676,7 +62697,7 @@
     </row>
     <row r="724">
       <c r="B724" t="s">
-        <v>12334</v>
+        <v>12336</v>
       </c>
       <c r="C724" t="s">
         <v>38</v>
@@ -62702,7 +62723,7 @@
     </row>
     <row r="725">
       <c r="B725" t="s">
-        <v>12335</v>
+        <v>12337</v>
       </c>
       <c r="C725" t="s">
         <v>38</v>
@@ -62728,7 +62749,7 @@
     </row>
     <row r="726">
       <c r="B726" t="s">
-        <v>12336</v>
+        <v>12338</v>
       </c>
       <c r="C726" t="s">
         <v>38</v>
@@ -62754,7 +62775,7 @@
     </row>
     <row r="727">
       <c r="B727" t="s">
-        <v>12337</v>
+        <v>12339</v>
       </c>
       <c r="C727" t="s">
         <v>38</v>
@@ -62780,7 +62801,7 @@
     </row>
     <row r="728">
       <c r="B728" t="s">
-        <v>12338</v>
+        <v>12340</v>
       </c>
       <c r="C728" t="s">
         <v>38</v>
@@ -62806,7 +62827,7 @@
     </row>
     <row r="729">
       <c r="B729" t="s">
-        <v>12339</v>
+        <v>12341</v>
       </c>
       <c r="C729" t="s">
         <v>38</v>
@@ -62832,7 +62853,7 @@
     </row>
     <row r="730">
       <c r="B730" t="s">
-        <v>12340</v>
+        <v>12342</v>
       </c>
       <c r="C730" t="s">
         <v>38</v>
@@ -62858,7 +62879,7 @@
     </row>
     <row r="731">
       <c r="B731" t="s">
-        <v>12341</v>
+        <v>12343</v>
       </c>
       <c r="C731" t="s">
         <v>38</v>
@@ -62884,7 +62905,7 @@
     </row>
     <row r="732">
       <c r="B732" t="s">
-        <v>12342</v>
+        <v>12344</v>
       </c>
       <c r="C732" t="s">
         <v>38</v>
@@ -62910,7 +62931,7 @@
     </row>
     <row r="733">
       <c r="B733" t="s">
-        <v>12343</v>
+        <v>12345</v>
       </c>
       <c r="C733" t="s">
         <v>38</v>
@@ -62936,7 +62957,7 @@
     </row>
     <row r="734">
       <c r="B734" t="s">
-        <v>12344</v>
+        <v>12346</v>
       </c>
       <c r="C734" t="s">
         <v>38</v>
@@ -62962,7 +62983,7 @@
     </row>
     <row r="735">
       <c r="B735" t="s">
-        <v>12345</v>
+        <v>12347</v>
       </c>
       <c r="C735" t="s">
         <v>38</v>
@@ -62988,7 +63009,7 @@
     </row>
     <row r="736">
       <c r="B736" t="s">
-        <v>12346</v>
+        <v>12348</v>
       </c>
       <c r="C736" t="s">
         <v>38</v>
@@ -63014,7 +63035,7 @@
     </row>
     <row r="737">
       <c r="B737" t="s">
-        <v>12347</v>
+        <v>12349</v>
       </c>
       <c r="C737" t="s">
         <v>38</v>
@@ -63040,7 +63061,7 @@
     </row>
     <row r="738">
       <c r="B738" t="s">
-        <v>12348</v>
+        <v>12350</v>
       </c>
       <c r="C738" t="s">
         <v>38</v>
@@ -63066,7 +63087,7 @@
     </row>
     <row r="739">
       <c r="B739" t="s">
-        <v>12349</v>
+        <v>12351</v>
       </c>
       <c r="C739" t="s">
         <v>38</v>
@@ -63092,7 +63113,7 @@
     </row>
     <row r="740">
       <c r="B740" t="s">
-        <v>12350</v>
+        <v>12352</v>
       </c>
       <c r="C740" t="s">
         <v>38</v>
@@ -63118,7 +63139,7 @@
     </row>
     <row r="741">
       <c r="B741" t="s">
-        <v>12351</v>
+        <v>12353</v>
       </c>
       <c r="C741" t="s">
         <v>38</v>
@@ -63144,7 +63165,7 @@
     </row>
     <row r="742">
       <c r="B742" t="s">
-        <v>12352</v>
+        <v>12354</v>
       </c>
       <c r="C742" t="s">
         <v>38</v>
@@ -63170,7 +63191,7 @@
     </row>
     <row r="743">
       <c r="B743" t="s">
-        <v>12353</v>
+        <v>12355</v>
       </c>
       <c r="C743" t="s">
         <v>38</v>
@@ -63196,7 +63217,7 @@
     </row>
     <row r="744">
       <c r="B744" t="s">
-        <v>12354</v>
+        <v>12356</v>
       </c>
       <c r="C744" t="s">
         <v>38</v>
@@ -63222,7 +63243,7 @@
     </row>
     <row r="745">
       <c r="B745" t="s">
-        <v>12355</v>
+        <v>12357</v>
       </c>
       <c r="C745" t="s">
         <v>38</v>
@@ -63248,7 +63269,7 @@
     </row>
     <row r="746">
       <c r="B746" t="s">
-        <v>12356</v>
+        <v>12358</v>
       </c>
       <c r="C746" t="s">
         <v>38</v>
@@ -63274,7 +63295,7 @@
     </row>
     <row r="747">
       <c r="B747" t="s">
-        <v>12357</v>
+        <v>12359</v>
       </c>
       <c r="C747" t="s">
         <v>38</v>
@@ -63300,7 +63321,7 @@
     </row>
     <row r="748">
       <c r="B748" t="s">
-        <v>12358</v>
+        <v>12360</v>
       </c>
       <c r="C748" t="s">
         <v>38</v>
@@ -63326,7 +63347,7 @@
     </row>
     <row r="749">
       <c r="B749" t="s">
-        <v>12359</v>
+        <v>12361</v>
       </c>
       <c r="C749" t="s">
         <v>38</v>
@@ -63352,7 +63373,7 @@
     </row>
     <row r="750">
       <c r="B750" t="s">
-        <v>12360</v>
+        <v>12362</v>
       </c>
       <c r="C750" t="s">
         <v>38</v>
@@ -63378,7 +63399,7 @@
     </row>
     <row r="751">
       <c r="B751" t="s">
-        <v>12361</v>
+        <v>12363</v>
       </c>
       <c r="C751" t="s">
         <v>38</v>
@@ -63390,24 +63411,24 @@
         <v>45</v>
       </c>
       <c r="F751" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G751" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H751" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I751" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="752">
       <c r="B752" t="s">
-        <v>12362</v>
+        <v>12285</v>
       </c>
       <c r="C752" t="s">
-        <v>38</v>
+        <v>1594</v>
       </c>
       <c r="D752" t="s">
         <v>44</v>
@@ -63416,131 +63437,131 @@
         <v>45</v>
       </c>
       <c r="F752" t="s">
-        <v>390</v>
+        <v>1294</v>
       </c>
       <c r="G752" t="s">
-        <v>284</v>
+        <v>1294</v>
       </c>
       <c r="H752" t="s">
-        <v>284</v>
+        <v>1294</v>
       </c>
       <c r="I752" t="s">
-        <v>284</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="753">
       <c r="B753" t="s">
-        <v>12363</v>
+        <v>12101</v>
       </c>
       <c r="C753" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D753" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E753" t="s">
         <v>45</v>
       </c>
       <c r="F753" t="s">
-        <v>47</v>
+        <v>12102</v>
       </c>
       <c r="G753" t="s">
-        <v>47</v>
+        <v>12102</v>
       </c>
       <c r="H753" t="s">
-        <v>47</v>
+        <v>12102</v>
       </c>
       <c r="I753" t="s">
-        <v>47</v>
+        <v>12102</v>
       </c>
     </row>
     <row r="754">
       <c r="B754" t="s">
-        <v>12285</v>
+        <v>12289</v>
       </c>
       <c r="C754" t="s">
-        <v>1594</v>
+        <v>40</v>
       </c>
       <c r="D754" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E754" t="s">
         <v>45</v>
       </c>
       <c r="F754" t="s">
-        <v>1294</v>
+        <v>12294</v>
       </c>
       <c r="G754" t="s">
-        <v>1294</v>
+        <v>12102</v>
       </c>
       <c r="H754" t="s">
-        <v>1294</v>
+        <v>12102</v>
       </c>
       <c r="I754" t="s">
-        <v>1294</v>
+        <v>12102</v>
       </c>
     </row>
     <row r="755">
       <c r="B755" t="s">
-        <v>12101</v>
+        <v>12364</v>
       </c>
       <c r="C755" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D755" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E755" t="s">
         <v>45</v>
       </c>
       <c r="F755" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="G755" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="H755" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="I755" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="756">
       <c r="B756" t="s">
-        <v>12289</v>
+        <v>12365</v>
       </c>
       <c r="C756" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D756" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E756" t="s">
         <v>45</v>
       </c>
       <c r="F756" t="s">
-        <v>12294</v>
+        <v>390</v>
       </c>
       <c r="G756" t="s">
-        <v>12102</v>
+        <v>284</v>
       </c>
       <c r="H756" t="s">
-        <v>12102</v>
+        <v>284</v>
       </c>
       <c r="I756" t="s">
-        <v>12102</v>
+        <v>284</v>
       </c>
     </row>
     <row r="757">
       <c r="B757" t="s">
-        <v>12364</v>
+        <v>12366</v>
       </c>
       <c r="C757" t="s">
         <v>38</v>
       </c>
       <c r="D757" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E757" t="s">
         <v>45</v>
@@ -63560,7 +63581,7 @@
     </row>
     <row r="758">
       <c r="B758" t="s">
-        <v>12365</v>
+        <v>12367</v>
       </c>
       <c r="C758" t="s">
         <v>38</v>
@@ -63575,24 +63596,24 @@
         <v>390</v>
       </c>
       <c r="G758" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="H758" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="I758" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
     </row>
     <row r="759">
       <c r="B759" t="s">
-        <v>12366</v>
+        <v>12368</v>
       </c>
       <c r="C759" t="s">
         <v>38</v>
       </c>
       <c r="D759" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E759" t="s">
         <v>45</v>
@@ -63612,7 +63633,7 @@
     </row>
     <row r="760">
       <c r="B760" t="s">
-        <v>12367</v>
+        <v>12369</v>
       </c>
       <c r="C760" t="s">
         <v>38</v>
@@ -63627,24 +63648,24 @@
         <v>390</v>
       </c>
       <c r="G760" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="H760" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="I760" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
     </row>
     <row r="761">
       <c r="B761" t="s">
-        <v>12368</v>
+        <v>12370</v>
       </c>
       <c r="C761" t="s">
         <v>38</v>
       </c>
       <c r="D761" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E761" t="s">
         <v>45</v>
@@ -63664,7 +63685,7 @@
     </row>
     <row r="762">
       <c r="B762" t="s">
-        <v>12369</v>
+        <v>12371</v>
       </c>
       <c r="C762" t="s">
         <v>38</v>
@@ -63679,24 +63700,24 @@
         <v>390</v>
       </c>
       <c r="G762" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="H762" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="I762" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
     </row>
     <row r="763">
       <c r="B763" t="s">
-        <v>12370</v>
+        <v>12372</v>
       </c>
       <c r="C763" t="s">
         <v>38</v>
       </c>
       <c r="D763" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E763" t="s">
         <v>45</v>
@@ -63716,7 +63737,7 @@
     </row>
     <row r="764">
       <c r="B764" t="s">
-        <v>12371</v>
+        <v>12373</v>
       </c>
       <c r="C764" t="s">
         <v>38</v>
@@ -63731,24 +63752,24 @@
         <v>390</v>
       </c>
       <c r="G764" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="H764" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
       <c r="I764" t="s">
-        <v>390</v>
+        <v>284</v>
       </c>
     </row>
     <row r="765">
       <c r="B765" t="s">
-        <v>12372</v>
+        <v>12374</v>
       </c>
       <c r="C765" t="s">
         <v>38</v>
       </c>
       <c r="D765" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E765" t="s">
         <v>45</v>
@@ -63768,7 +63789,7 @@
     </row>
     <row r="766">
       <c r="B766" t="s">
-        <v>12373</v>
+        <v>12375</v>
       </c>
       <c r="C766" t="s">
         <v>38</v>
@@ -63783,19 +63804,119 @@
         <v>390</v>
       </c>
       <c r="G766" t="s">
+        <v>284</v>
+      </c>
+      <c r="H766" t="s">
+        <v>284</v>
+      </c>
+      <c r="I766" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="B767" t="s">
+        <v>12377</v>
+      </c>
+      <c r="C767" t="s">
+        <v>38</v>
+      </c>
+      <c r="D767" t="s">
+        <v>44</v>
+      </c>
+      <c r="E767" t="s">
+        <v>45</v>
+      </c>
+      <c r="F767" t="s">
+        <v>50</v>
+      </c>
+      <c r="G767" t="s">
+        <v>50</v>
+      </c>
+      <c r="H767" t="s">
+        <v>50</v>
+      </c>
+      <c r="I767" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="B768" t="s">
+        <v>12378</v>
+      </c>
+      <c r="C768" t="s">
+        <v>38</v>
+      </c>
+      <c r="D768" t="s">
+        <v>44</v>
+      </c>
+      <c r="E768" t="s">
+        <v>45</v>
+      </c>
+      <c r="F768" t="s">
         <v>390</v>
       </c>
-      <c r="H766" t="s">
+      <c r="G768" t="s">
+        <v>284</v>
+      </c>
+      <c r="H768" t="s">
+        <v>284</v>
+      </c>
+      <c r="I768" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="B769" t="s">
+        <v>12379</v>
+      </c>
+      <c r="C769" t="s">
+        <v>38</v>
+      </c>
+      <c r="D769" t="s">
+        <v>44</v>
+      </c>
+      <c r="E769" t="s">
+        <v>45</v>
+      </c>
+      <c r="F769" t="s">
+        <v>50</v>
+      </c>
+      <c r="G769" t="s">
+        <v>50</v>
+      </c>
+      <c r="H769" t="s">
+        <v>50</v>
+      </c>
+      <c r="I769" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="B770" t="s">
+        <v>12380</v>
+      </c>
+      <c r="C770" t="s">
+        <v>38</v>
+      </c>
+      <c r="D770" t="s">
+        <v>44</v>
+      </c>
+      <c r="E770" t="s">
+        <v>45</v>
+      </c>
+      <c r="F770" t="s">
         <v>390</v>
       </c>
-      <c r="I766" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="767"/>
-    <row r="768"/>
-    <row r="769"/>
-    <row r="770"/>
+      <c r="G770" t="s">
+        <v>284</v>
+      </c>
+      <c r="H770" t="s">
+        <v>284</v>
+      </c>
+      <c r="I770" t="s">
+        <v>284</v>
+      </c>
+    </row>
     <row r="771"/>
     <row r="772"/>
     <row r="773"/>

</xml_diff>

<commit_message>
add all congelar scripts
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6457780" uniqueCount="12374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6485848" uniqueCount="12376">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -41926,6 +41926,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4177</t>
   </si>
 </sst>
 </file>
@@ -63792,8 +63798,58 @@
         <v>390</v>
       </c>
     </row>
-    <row r="767"/>
-    <row r="768"/>
+    <row r="767">
+      <c r="B767" t="s">
+        <v>12374</v>
+      </c>
+      <c r="C767" t="s">
+        <v>38</v>
+      </c>
+      <c r="D767" t="s">
+        <v>44</v>
+      </c>
+      <c r="E767" t="s">
+        <v>45</v>
+      </c>
+      <c r="F767" t="s">
+        <v>50</v>
+      </c>
+      <c r="G767" t="s">
+        <v>50</v>
+      </c>
+      <c r="H767" t="s">
+        <v>50</v>
+      </c>
+      <c r="I767" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="B768" t="s">
+        <v>12375</v>
+      </c>
+      <c r="C768" t="s">
+        <v>38</v>
+      </c>
+      <c r="D768" t="s">
+        <v>44</v>
+      </c>
+      <c r="E768" t="s">
+        <v>45</v>
+      </c>
+      <c r="F768" t="s">
+        <v>50</v>
+      </c>
+      <c r="G768" t="s">
+        <v>50</v>
+      </c>
+      <c r="H768" t="s">
+        <v>50</v>
+      </c>
+      <c r="I768" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="769"/>
     <row r="770"/>
     <row r="771"/>

</xml_diff>

<commit_message>
Fix Higiene screen bug
</commit_message>
<xml_diff>
--- a/Px4/TouchGFX/assets/texts/texts.xlsx
+++ b/Px4/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6541504" uniqueCount="12381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6560252" uniqueCount="12381">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -63477,33 +63477,33 @@
     </row>
     <row r="754">
       <c r="B754" t="s">
-        <v>12289</v>
+        <v>12364</v>
       </c>
       <c r="C754" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D754" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E754" t="s">
         <v>45</v>
       </c>
       <c r="F754" t="s">
-        <v>12294</v>
+        <v>50</v>
       </c>
       <c r="G754" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="H754" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
       <c r="I754" t="s">
-        <v>12102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="755">
       <c r="B755" t="s">
-        <v>12364</v>
+        <v>12365</v>
       </c>
       <c r="C755" t="s">
         <v>38</v>
@@ -63515,21 +63515,21 @@
         <v>45</v>
       </c>
       <c r="F755" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G755" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H755" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I755" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="756">
       <c r="B756" t="s">
-        <v>12365</v>
+        <v>12366</v>
       </c>
       <c r="C756" t="s">
         <v>38</v>
@@ -63541,21 +63541,21 @@
         <v>45</v>
       </c>
       <c r="F756" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G756" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H756" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I756" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="757">
       <c r="B757" t="s">
-        <v>12366</v>
+        <v>12367</v>
       </c>
       <c r="C757" t="s">
         <v>38</v>
@@ -63567,21 +63567,21 @@
         <v>45</v>
       </c>
       <c r="F757" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G757" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H757" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I757" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="758">
       <c r="B758" t="s">
-        <v>12367</v>
+        <v>12368</v>
       </c>
       <c r="C758" t="s">
         <v>38</v>
@@ -63593,21 +63593,21 @@
         <v>45</v>
       </c>
       <c r="F758" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G758" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H758" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I758" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="759">
       <c r="B759" t="s">
-        <v>12368</v>
+        <v>12369</v>
       </c>
       <c r="C759" t="s">
         <v>38</v>
@@ -63619,21 +63619,21 @@
         <v>45</v>
       </c>
       <c r="F759" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G759" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H759" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I759" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="760">
       <c r="B760" t="s">
-        <v>12369</v>
+        <v>12370</v>
       </c>
       <c r="C760" t="s">
         <v>38</v>
@@ -63645,21 +63645,21 @@
         <v>45</v>
       </c>
       <c r="F760" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G760" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H760" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I760" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="761">
       <c r="B761" t="s">
-        <v>12370</v>
+        <v>12371</v>
       </c>
       <c r="C761" t="s">
         <v>38</v>
@@ -63671,21 +63671,21 @@
         <v>45</v>
       </c>
       <c r="F761" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G761" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H761" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I761" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="762">
       <c r="B762" t="s">
-        <v>12371</v>
+        <v>12372</v>
       </c>
       <c r="C762" t="s">
         <v>38</v>
@@ -63697,21 +63697,21 @@
         <v>45</v>
       </c>
       <c r="F762" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G762" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H762" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I762" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="763">
       <c r="B763" t="s">
-        <v>12372</v>
+        <v>12373</v>
       </c>
       <c r="C763" t="s">
         <v>38</v>
@@ -63723,21 +63723,21 @@
         <v>45</v>
       </c>
       <c r="F763" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G763" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H763" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I763" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="764">
       <c r="B764" t="s">
-        <v>12373</v>
+        <v>12374</v>
       </c>
       <c r="C764" t="s">
         <v>38</v>
@@ -63749,21 +63749,21 @@
         <v>45</v>
       </c>
       <c r="F764" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G764" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H764" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I764" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="765">
       <c r="B765" t="s">
-        <v>12374</v>
+        <v>12375</v>
       </c>
       <c r="C765" t="s">
         <v>38</v>
@@ -63775,21 +63775,21 @@
         <v>45</v>
       </c>
       <c r="F765" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G765" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H765" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I765" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="766">
       <c r="B766" t="s">
-        <v>12375</v>
+        <v>12377</v>
       </c>
       <c r="C766" t="s">
         <v>38</v>
@@ -63801,21 +63801,21 @@
         <v>45</v>
       </c>
       <c r="F766" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G766" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H766" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I766" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="767">
       <c r="B767" t="s">
-        <v>12377</v>
+        <v>12378</v>
       </c>
       <c r="C767" t="s">
         <v>38</v>
@@ -63827,21 +63827,21 @@
         <v>45</v>
       </c>
       <c r="F767" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G767" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H767" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I767" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="768">
       <c r="B768" t="s">
-        <v>12378</v>
+        <v>12379</v>
       </c>
       <c r="C768" t="s">
         <v>38</v>
@@ -63853,21 +63853,21 @@
         <v>45</v>
       </c>
       <c r="F768" t="s">
-        <v>390</v>
+        <v>50</v>
       </c>
       <c r="G768" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="H768" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
       <c r="I768" t="s">
-        <v>284</v>
+        <v>50</v>
       </c>
     </row>
     <row r="769">
       <c r="B769" t="s">
-        <v>12379</v>
+        <v>12380</v>
       </c>
       <c r="C769" t="s">
         <v>38</v>
@@ -63879,42 +63879,42 @@
         <v>45</v>
       </c>
       <c r="F769" t="s">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="G769" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="H769" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="I769" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
     </row>
     <row r="770">
       <c r="B770" t="s">
-        <v>12380</v>
+        <v>12289</v>
       </c>
       <c r="C770" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D770" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E770" t="s">
         <v>45</v>
       </c>
       <c r="F770" t="s">
-        <v>390</v>
+        <v>12294</v>
       </c>
       <c r="G770" t="s">
-        <v>284</v>
+        <v>12102</v>
       </c>
       <c r="H770" t="s">
-        <v>284</v>
+        <v>12102</v>
       </c>
       <c r="I770" t="s">
-        <v>284</v>
+        <v>12102</v>
       </c>
     </row>
     <row r="771"/>

</xml_diff>